<commit_message>
Update modified files including reports, dashboard, and database logic
</commit_message>
<xml_diff>
--- a/daily-attendance.xlsx
+++ b/daily-attendance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\scan-admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\scan-admin-panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F54851A-0313-41EB-AD44-423156F97D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192CCAEA-7286-4C55-9B66-F14AC7126F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2810119D-446A-4390-98EB-179F470E2279}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="90">
   <si>
     <t>School Form 2 (SF2) Daily Attendance Report of Learners</t>
   </si>
@@ -435,9 +435,6 @@
     <t>d.2. Armed conflict (incl. Tribal wars &amp; clanfeuds)</t>
   </si>
   <si>
-    <t xml:space="preserve">                      ALONA M. MANALO</t>
-  </si>
-  <si>
     <t xml:space="preserve">                          (Signature of Teacher over Printed Name)</t>
   </si>
   <si>
@@ -456,13 +453,13 @@
     <t>e.1. Child labor, work</t>
   </si>
   <si>
-    <t xml:space="preserve">          DR. JOSE ALEJANDRO R. BELEN</t>
-  </si>
-  <si>
     <t>f. Others</t>
   </si>
   <si>
     <t xml:space="preserve"> (Signature of School Head over Printed Name)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         </t>
   </si>
 </sst>
 </file>
@@ -1840,7 +1837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="243">
+  <cellXfs count="245">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2192,6 +2189,351 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="87"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="87"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2210,353 +2552,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="87"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="87"/>
-    </xf>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3074,8 +3077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D90EB3-0037-48DC-8872-1162DFAD7304}">
   <dimension ref="A1:AK106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O78" zoomScale="119" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="AB79" sqref="AB79:AG80"/>
+    <sheetView tabSelected="1" topLeftCell="Q94" zoomScale="101" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="AF101" sqref="AF101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.36328125" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -3133,84 +3136,84 @@
       <c r="AJ1" s="4"/>
     </row>
     <row r="2" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="233" t="s">
+      <c r="A2" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="233"/>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233"/>
-      <c r="H2" s="233"/>
-      <c r="I2" s="233"/>
-      <c r="J2" s="233"/>
-      <c r="K2" s="233"/>
-      <c r="L2" s="233"/>
-      <c r="M2" s="233"/>
-      <c r="N2" s="233"/>
-      <c r="O2" s="233"/>
-      <c r="P2" s="233"/>
-      <c r="Q2" s="233"/>
-      <c r="R2" s="233"/>
-      <c r="S2" s="233"/>
-      <c r="T2" s="233"/>
-      <c r="U2" s="233"/>
-      <c r="V2" s="233"/>
-      <c r="W2" s="233"/>
-      <c r="X2" s="233"/>
-      <c r="Y2" s="233"/>
-      <c r="Z2" s="233"/>
-      <c r="AA2" s="233"/>
-      <c r="AB2" s="233"/>
-      <c r="AC2" s="233"/>
-      <c r="AD2" s="233"/>
-      <c r="AE2" s="233"/>
-      <c r="AF2" s="233"/>
-      <c r="AG2" s="233"/>
-      <c r="AH2" s="233"/>
-      <c r="AI2" s="233"/>
-      <c r="AJ2" s="233"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="123"/>
+      <c r="T2" s="123"/>
+      <c r="U2" s="123"/>
+      <c r="V2" s="123"/>
+      <c r="W2" s="123"/>
+      <c r="X2" s="123"/>
+      <c r="Y2" s="123"/>
+      <c r="Z2" s="123"/>
+      <c r="AA2" s="123"/>
+      <c r="AB2" s="123"/>
+      <c r="AC2" s="123"/>
+      <c r="AD2" s="123"/>
+      <c r="AE2" s="123"/>
+      <c r="AF2" s="123"/>
+      <c r="AG2" s="123"/>
+      <c r="AH2" s="123"/>
+      <c r="AI2" s="123"/>
+      <c r="AJ2" s="123"/>
     </row>
     <row r="3" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="168"/>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="168"/>
-      <c r="J3" s="168"/>
-      <c r="K3" s="168"/>
-      <c r="L3" s="168"/>
-      <c r="M3" s="168"/>
-      <c r="N3" s="168"/>
-      <c r="O3" s="168"/>
-      <c r="P3" s="168"/>
-      <c r="Q3" s="168"/>
-      <c r="R3" s="168"/>
-      <c r="S3" s="168"/>
-      <c r="T3" s="168"/>
-      <c r="U3" s="168"/>
-      <c r="V3" s="168"/>
-      <c r="W3" s="168"/>
-      <c r="X3" s="168"/>
-      <c r="Y3" s="168"/>
-      <c r="Z3" s="168"/>
-      <c r="AA3" s="168"/>
-      <c r="AB3" s="168"/>
-      <c r="AC3" s="168"/>
-      <c r="AD3" s="168"/>
-      <c r="AE3" s="168"/>
-      <c r="AF3" s="168"/>
-      <c r="AG3" s="168"/>
-      <c r="AH3" s="168"/>
-      <c r="AI3" s="168"/>
-      <c r="AJ3" s="168"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124"/>
+      <c r="N3" s="124"/>
+      <c r="O3" s="124"/>
+      <c r="P3" s="124"/>
+      <c r="Q3" s="124"/>
+      <c r="R3" s="124"/>
+      <c r="S3" s="124"/>
+      <c r="T3" s="124"/>
+      <c r="U3" s="124"/>
+      <c r="V3" s="124"/>
+      <c r="W3" s="124"/>
+      <c r="X3" s="124"/>
+      <c r="Y3" s="124"/>
+      <c r="Z3" s="124"/>
+      <c r="AA3" s="124"/>
+      <c r="AB3" s="124"/>
+      <c r="AC3" s="124"/>
+      <c r="AD3" s="124"/>
+      <c r="AE3" s="124"/>
+      <c r="AF3" s="124"/>
+      <c r="AG3" s="124"/>
+      <c r="AH3" s="124"/>
+      <c r="AI3" s="124"/>
+      <c r="AJ3" s="124"/>
     </row>
     <row r="4" spans="1:36" ht="6.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
@@ -3293,11 +3296,11 @@
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="234">
+      <c r="C6" s="125">
         <v>600030</v>
       </c>
-      <c r="D6" s="235"/>
-      <c r="E6" s="236"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="127"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
@@ -3305,27 +3308,27 @@
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="234"/>
-      <c r="L6" s="235"/>
-      <c r="M6" s="235"/>
-      <c r="N6" s="235"/>
-      <c r="O6" s="236"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="126"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="127"/>
       <c r="P6" s="8"/>
-      <c r="Q6" s="237" t="s">
+      <c r="Q6" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="R6" s="237"/>
-      <c r="S6" s="237"/>
-      <c r="T6" s="237"/>
-      <c r="U6" s="237"/>
-      <c r="V6" s="237"/>
-      <c r="W6" s="238"/>
-      <c r="X6" s="234"/>
-      <c r="Y6" s="235"/>
-      <c r="Z6" s="235"/>
-      <c r="AA6" s="235"/>
-      <c r="AB6" s="235"/>
-      <c r="AC6" s="236"/>
+      <c r="R6" s="128"/>
+      <c r="S6" s="128"/>
+      <c r="T6" s="128"/>
+      <c r="U6" s="128"/>
+      <c r="V6" s="128"/>
+      <c r="W6" s="129"/>
+      <c r="X6" s="125"/>
+      <c r="Y6" s="126"/>
+      <c r="Z6" s="126"/>
+      <c r="AA6" s="126"/>
+      <c r="AB6" s="126"/>
+      <c r="AC6" s="127"/>
       <c r="AD6" s="8"/>
       <c r="AE6" s="8"/>
       <c r="AF6" s="8"/>
@@ -3377,98 +3380,98 @@
       <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="239" t="s">
+      <c r="C8" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="240"/>
-      <c r="E8" s="240"/>
-      <c r="F8" s="240"/>
-      <c r="G8" s="240"/>
-      <c r="H8" s="240"/>
-      <c r="I8" s="240"/>
-      <c r="J8" s="240"/>
-      <c r="K8" s="240"/>
-      <c r="L8" s="240"/>
-      <c r="M8" s="240"/>
-      <c r="N8" s="240"/>
-      <c r="O8" s="241"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
+      <c r="H8" s="131"/>
+      <c r="I8" s="131"/>
+      <c r="J8" s="131"/>
+      <c r="K8" s="131"/>
+      <c r="L8" s="131"/>
+      <c r="M8" s="131"/>
+      <c r="N8" s="131"/>
+      <c r="O8" s="132"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
-      <c r="T8" s="237" t="s">
+      <c r="T8" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="237"/>
-      <c r="V8" s="237"/>
-      <c r="W8" s="238"/>
-      <c r="X8" s="234"/>
-      <c r="Y8" s="236"/>
-      <c r="Z8" s="242" t="s">
+      <c r="U8" s="128"/>
+      <c r="V8" s="128"/>
+      <c r="W8" s="129"/>
+      <c r="X8" s="125"/>
+      <c r="Y8" s="127"/>
+      <c r="Z8" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="AA8" s="237"/>
-      <c r="AB8" s="238"/>
-      <c r="AC8" s="234"/>
-      <c r="AD8" s="235"/>
-      <c r="AE8" s="235"/>
-      <c r="AF8" s="235"/>
-      <c r="AG8" s="235"/>
-      <c r="AH8" s="236"/>
+      <c r="AA8" s="128"/>
+      <c r="AB8" s="129"/>
+      <c r="AC8" s="125"/>
+      <c r="AD8" s="126"/>
+      <c r="AE8" s="126"/>
+      <c r="AF8" s="126"/>
+      <c r="AG8" s="126"/>
+      <c r="AH8" s="127"/>
       <c r="AI8" s="9"/>
       <c r="AJ8" s="9"/>
     </row>
     <row r="9" spans="1:36" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:36" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="208" t="s">
+      <c r="A10" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="209"/>
-      <c r="C10" s="210"/>
-      <c r="D10" s="217" t="s">
+      <c r="B10" s="135"/>
+      <c r="C10" s="136"/>
+      <c r="D10" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="218"/>
-      <c r="F10" s="218"/>
-      <c r="G10" s="218"/>
-      <c r="H10" s="218"/>
-      <c r="I10" s="218"/>
-      <c r="J10" s="218"/>
-      <c r="K10" s="218"/>
-      <c r="L10" s="218"/>
-      <c r="M10" s="218"/>
-      <c r="N10" s="218"/>
-      <c r="O10" s="218"/>
-      <c r="P10" s="218"/>
-      <c r="Q10" s="218"/>
-      <c r="R10" s="218"/>
-      <c r="S10" s="218"/>
-      <c r="T10" s="218"/>
-      <c r="U10" s="218"/>
-      <c r="V10" s="218"/>
-      <c r="W10" s="218"/>
-      <c r="X10" s="218"/>
-      <c r="Y10" s="218"/>
-      <c r="Z10" s="218"/>
-      <c r="AA10" s="218"/>
-      <c r="AB10" s="219"/>
-      <c r="AC10" s="220" t="s">
+      <c r="E10" s="144"/>
+      <c r="F10" s="144"/>
+      <c r="G10" s="144"/>
+      <c r="H10" s="144"/>
+      <c r="I10" s="144"/>
+      <c r="J10" s="144"/>
+      <c r="K10" s="144"/>
+      <c r="L10" s="144"/>
+      <c r="M10" s="144"/>
+      <c r="N10" s="144"/>
+      <c r="O10" s="144"/>
+      <c r="P10" s="144"/>
+      <c r="Q10" s="144"/>
+      <c r="R10" s="144"/>
+      <c r="S10" s="144"/>
+      <c r="T10" s="144"/>
+      <c r="U10" s="144"/>
+      <c r="V10" s="144"/>
+      <c r="W10" s="144"/>
+      <c r="X10" s="144"/>
+      <c r="Y10" s="144"/>
+      <c r="Z10" s="144"/>
+      <c r="AA10" s="144"/>
+      <c r="AB10" s="145"/>
+      <c r="AC10" s="146" t="s">
         <v>11</v>
       </c>
-      <c r="AD10" s="220"/>
-      <c r="AE10" s="222" t="s">
+      <c r="AD10" s="146"/>
+      <c r="AE10" s="148" t="s">
         <v>12</v>
       </c>
-      <c r="AF10" s="223"/>
-      <c r="AG10" s="223"/>
-      <c r="AH10" s="223"/>
-      <c r="AI10" s="223"/>
-      <c r="AJ10" s="224"/>
+      <c r="AF10" s="149"/>
+      <c r="AG10" s="149"/>
+      <c r="AH10" s="149"/>
+      <c r="AI10" s="149"/>
+      <c r="AJ10" s="150"/>
     </row>
     <row r="11" spans="1:36" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="211"/>
-      <c r="B11" s="212"/>
-      <c r="C11" s="213"/>
+      <c r="A11" s="137"/>
+      <c r="B11" s="138"/>
+      <c r="C11" s="139"/>
       <c r="D11" s="113"/>
       <c r="E11" s="114"/>
       <c r="F11" s="114"/>
@@ -3494,19 +3497,19 @@
       <c r="Z11" s="116"/>
       <c r="AA11" s="116"/>
       <c r="AB11" s="117"/>
-      <c r="AC11" s="221"/>
-      <c r="AD11" s="221"/>
-      <c r="AE11" s="225"/>
-      <c r="AF11" s="226"/>
-      <c r="AG11" s="226"/>
-      <c r="AH11" s="226"/>
-      <c r="AI11" s="226"/>
-      <c r="AJ11" s="227"/>
+      <c r="AC11" s="147"/>
+      <c r="AD11" s="147"/>
+      <c r="AE11" s="151"/>
+      <c r="AF11" s="152"/>
+      <c r="AG11" s="152"/>
+      <c r="AH11" s="152"/>
+      <c r="AI11" s="152"/>
+      <c r="AJ11" s="153"/>
     </row>
     <row r="12" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="211"/>
-      <c r="B12" s="212"/>
-      <c r="C12" s="213"/>
+      <c r="A12" s="137"/>
+      <c r="B12" s="138"/>
+      <c r="C12" s="139"/>
       <c r="D12" s="11" t="s">
         <v>13</v>
       </c>
@@ -3582,23 +3585,23 @@
       <c r="AB12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AC12" s="231" t="s">
+      <c r="AC12" s="157" t="s">
         <v>18</v>
       </c>
-      <c r="AD12" s="206" t="s">
+      <c r="AD12" s="162" t="s">
         <v>19</v>
       </c>
-      <c r="AE12" s="225"/>
-      <c r="AF12" s="226"/>
-      <c r="AG12" s="226"/>
-      <c r="AH12" s="226"/>
-      <c r="AI12" s="226"/>
-      <c r="AJ12" s="227"/>
+      <c r="AE12" s="151"/>
+      <c r="AF12" s="152"/>
+      <c r="AG12" s="152"/>
+      <c r="AH12" s="152"/>
+      <c r="AI12" s="152"/>
+      <c r="AJ12" s="153"/>
     </row>
     <row r="13" spans="1:36" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="214"/>
-      <c r="B13" s="215"/>
-      <c r="C13" s="216"/>
+      <c r="A13" s="140"/>
+      <c r="B13" s="141"/>
+      <c r="C13" s="142"/>
       <c r="D13" s="13"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -3624,14 +3627,14 @@
       <c r="Z13" s="14"/>
       <c r="AA13" s="17"/>
       <c r="AB13" s="15"/>
-      <c r="AC13" s="232"/>
-      <c r="AD13" s="207"/>
-      <c r="AE13" s="228"/>
-      <c r="AF13" s="229"/>
-      <c r="AG13" s="229"/>
-      <c r="AH13" s="229"/>
-      <c r="AI13" s="229"/>
-      <c r="AJ13" s="230"/>
+      <c r="AC13" s="158"/>
+      <c r="AD13" s="163"/>
+      <c r="AE13" s="154"/>
+      <c r="AF13" s="155"/>
+      <c r="AG13" s="155"/>
+      <c r="AH13" s="155"/>
+      <c r="AI13" s="155"/>
+      <c r="AJ13" s="156"/>
     </row>
     <row r="14" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="18">
@@ -3666,12 +3669,12 @@
       <c r="AB14" s="27"/>
       <c r="AC14" s="29"/>
       <c r="AD14" s="30"/>
-      <c r="AE14" s="200"/>
-      <c r="AF14" s="201"/>
-      <c r="AG14" s="201"/>
-      <c r="AH14" s="201"/>
-      <c r="AI14" s="201"/>
-      <c r="AJ14" s="202"/>
+      <c r="AE14" s="164"/>
+      <c r="AF14" s="165"/>
+      <c r="AG14" s="165"/>
+      <c r="AH14" s="165"/>
+      <c r="AI14" s="165"/>
+      <c r="AJ14" s="166"/>
     </row>
     <row r="15" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31">
@@ -3706,12 +3709,12 @@
       <c r="AB15" s="38"/>
       <c r="AC15" s="40"/>
       <c r="AD15" s="41"/>
-      <c r="AE15" s="198"/>
-      <c r="AF15" s="199"/>
-      <c r="AG15" s="199"/>
-      <c r="AH15" s="199"/>
-      <c r="AI15" s="199"/>
-      <c r="AJ15" s="197"/>
+      <c r="AE15" s="159"/>
+      <c r="AF15" s="160"/>
+      <c r="AG15" s="160"/>
+      <c r="AH15" s="160"/>
+      <c r="AI15" s="160"/>
+      <c r="AJ15" s="161"/>
     </row>
     <row r="16" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18">
@@ -3746,12 +3749,12 @@
       <c r="AB16" s="38"/>
       <c r="AC16" s="40"/>
       <c r="AD16" s="41"/>
-      <c r="AE16" s="198"/>
-      <c r="AF16" s="199"/>
-      <c r="AG16" s="199"/>
-      <c r="AH16" s="199"/>
-      <c r="AI16" s="199"/>
-      <c r="AJ16" s="197"/>
+      <c r="AE16" s="159"/>
+      <c r="AF16" s="160"/>
+      <c r="AG16" s="160"/>
+      <c r="AH16" s="160"/>
+      <c r="AI16" s="160"/>
+      <c r="AJ16" s="161"/>
     </row>
     <row r="17" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="31">
@@ -3786,12 +3789,12 @@
       <c r="AB17" s="38"/>
       <c r="AC17" s="40"/>
       <c r="AD17" s="41"/>
-      <c r="AE17" s="198"/>
-      <c r="AF17" s="199"/>
-      <c r="AG17" s="199"/>
-      <c r="AH17" s="199"/>
-      <c r="AI17" s="199"/>
-      <c r="AJ17" s="197"/>
+      <c r="AE17" s="159"/>
+      <c r="AF17" s="160"/>
+      <c r="AG17" s="160"/>
+      <c r="AH17" s="160"/>
+      <c r="AI17" s="160"/>
+      <c r="AJ17" s="161"/>
     </row>
     <row r="18" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18">
@@ -3826,12 +3829,12 @@
       <c r="AB18" s="38"/>
       <c r="AC18" s="40"/>
       <c r="AD18" s="41"/>
-      <c r="AE18" s="198"/>
-      <c r="AF18" s="199"/>
-      <c r="AG18" s="199"/>
-      <c r="AH18" s="199"/>
-      <c r="AI18" s="199"/>
-      <c r="AJ18" s="197"/>
+      <c r="AE18" s="159"/>
+      <c r="AF18" s="160"/>
+      <c r="AG18" s="160"/>
+      <c r="AH18" s="160"/>
+      <c r="AI18" s="160"/>
+      <c r="AJ18" s="161"/>
     </row>
     <row r="19" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="31">
@@ -3866,12 +3869,12 @@
       <c r="AB19" s="38"/>
       <c r="AC19" s="40"/>
       <c r="AD19" s="41"/>
-      <c r="AE19" s="198"/>
-      <c r="AF19" s="199"/>
-      <c r="AG19" s="199"/>
-      <c r="AH19" s="199"/>
-      <c r="AI19" s="199"/>
-      <c r="AJ19" s="197"/>
+      <c r="AE19" s="159"/>
+      <c r="AF19" s="160"/>
+      <c r="AG19" s="160"/>
+      <c r="AH19" s="160"/>
+      <c r="AI19" s="160"/>
+      <c r="AJ19" s="161"/>
     </row>
     <row r="20" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18">
@@ -3906,12 +3909,12 @@
       <c r="AB20" s="38"/>
       <c r="AC20" s="40"/>
       <c r="AD20" s="41"/>
-      <c r="AE20" s="198"/>
-      <c r="AF20" s="199"/>
-      <c r="AG20" s="199"/>
-      <c r="AH20" s="199"/>
-      <c r="AI20" s="199"/>
-      <c r="AJ20" s="197"/>
+      <c r="AE20" s="159"/>
+      <c r="AF20" s="160"/>
+      <c r="AG20" s="160"/>
+      <c r="AH20" s="160"/>
+      <c r="AI20" s="160"/>
+      <c r="AJ20" s="161"/>
     </row>
     <row r="21" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="31">
@@ -3946,12 +3949,12 @@
       <c r="AB21" s="38"/>
       <c r="AC21" s="40"/>
       <c r="AD21" s="41"/>
-      <c r="AE21" s="198"/>
-      <c r="AF21" s="199"/>
-      <c r="AG21" s="199"/>
-      <c r="AH21" s="199"/>
-      <c r="AI21" s="199"/>
-      <c r="AJ21" s="197"/>
+      <c r="AE21" s="159"/>
+      <c r="AF21" s="160"/>
+      <c r="AG21" s="160"/>
+      <c r="AH21" s="160"/>
+      <c r="AI21" s="160"/>
+      <c r="AJ21" s="161"/>
     </row>
     <row r="22" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18">
@@ -3986,12 +3989,12 @@
       <c r="AB22" s="38"/>
       <c r="AC22" s="40"/>
       <c r="AD22" s="41"/>
-      <c r="AE22" s="198"/>
-      <c r="AF22" s="199"/>
-      <c r="AG22" s="199"/>
-      <c r="AH22" s="199"/>
-      <c r="AI22" s="199"/>
-      <c r="AJ22" s="197"/>
+      <c r="AE22" s="159"/>
+      <c r="AF22" s="160"/>
+      <c r="AG22" s="160"/>
+      <c r="AH22" s="160"/>
+      <c r="AI22" s="160"/>
+      <c r="AJ22" s="161"/>
     </row>
     <row r="23" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="31">
@@ -4026,12 +4029,12 @@
       <c r="AB23" s="38"/>
       <c r="AC23" s="40"/>
       <c r="AD23" s="41"/>
-      <c r="AE23" s="198"/>
-      <c r="AF23" s="199"/>
-      <c r="AG23" s="199"/>
-      <c r="AH23" s="199"/>
-      <c r="AI23" s="199"/>
-      <c r="AJ23" s="197"/>
+      <c r="AE23" s="159"/>
+      <c r="AF23" s="160"/>
+      <c r="AG23" s="160"/>
+      <c r="AH23" s="160"/>
+      <c r="AI23" s="160"/>
+      <c r="AJ23" s="161"/>
     </row>
     <row r="24" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18">
@@ -4066,12 +4069,12 @@
       <c r="AB24" s="38"/>
       <c r="AC24" s="40"/>
       <c r="AD24" s="41"/>
-      <c r="AE24" s="198"/>
-      <c r="AF24" s="199"/>
-      <c r="AG24" s="199"/>
-      <c r="AH24" s="199"/>
-      <c r="AI24" s="199"/>
-      <c r="AJ24" s="197"/>
+      <c r="AE24" s="159"/>
+      <c r="AF24" s="160"/>
+      <c r="AG24" s="160"/>
+      <c r="AH24" s="160"/>
+      <c r="AI24" s="160"/>
+      <c r="AJ24" s="161"/>
     </row>
     <row r="25" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="31">
@@ -4106,12 +4109,12 @@
       <c r="AB25" s="38"/>
       <c r="AC25" s="40"/>
       <c r="AD25" s="41"/>
-      <c r="AE25" s="203"/>
-      <c r="AF25" s="204"/>
-      <c r="AG25" s="204"/>
-      <c r="AH25" s="204"/>
-      <c r="AI25" s="204"/>
-      <c r="AJ25" s="205"/>
+      <c r="AE25" s="170"/>
+      <c r="AF25" s="171"/>
+      <c r="AG25" s="171"/>
+      <c r="AH25" s="171"/>
+      <c r="AI25" s="171"/>
+      <c r="AJ25" s="172"/>
     </row>
     <row r="26" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18">
@@ -4146,12 +4149,12 @@
       <c r="AB26" s="38"/>
       <c r="AC26" s="40"/>
       <c r="AD26" s="41"/>
-      <c r="AE26" s="198"/>
-      <c r="AF26" s="199"/>
-      <c r="AG26" s="199"/>
-      <c r="AH26" s="199"/>
-      <c r="AI26" s="199"/>
-      <c r="AJ26" s="197"/>
+      <c r="AE26" s="159"/>
+      <c r="AF26" s="160"/>
+      <c r="AG26" s="160"/>
+      <c r="AH26" s="160"/>
+      <c r="AI26" s="160"/>
+      <c r="AJ26" s="161"/>
     </row>
     <row r="27" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="31">
@@ -4186,12 +4189,12 @@
       <c r="AB27" s="38"/>
       <c r="AC27" s="40"/>
       <c r="AD27" s="41"/>
-      <c r="AE27" s="198"/>
-      <c r="AF27" s="199"/>
-      <c r="AG27" s="199"/>
-      <c r="AH27" s="199"/>
-      <c r="AI27" s="199"/>
-      <c r="AJ27" s="197"/>
+      <c r="AE27" s="159"/>
+      <c r="AF27" s="160"/>
+      <c r="AG27" s="160"/>
+      <c r="AH27" s="160"/>
+      <c r="AI27" s="160"/>
+      <c r="AJ27" s="161"/>
     </row>
     <row r="28" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18">
@@ -4226,12 +4229,12 @@
       <c r="AB28" s="38"/>
       <c r="AC28" s="40"/>
       <c r="AD28" s="41"/>
-      <c r="AE28" s="198"/>
-      <c r="AF28" s="199"/>
-      <c r="AG28" s="199"/>
-      <c r="AH28" s="199"/>
-      <c r="AI28" s="199"/>
-      <c r="AJ28" s="197"/>
+      <c r="AE28" s="159"/>
+      <c r="AF28" s="160"/>
+      <c r="AG28" s="160"/>
+      <c r="AH28" s="160"/>
+      <c r="AI28" s="160"/>
+      <c r="AJ28" s="161"/>
     </row>
     <row r="29" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="31">
@@ -4266,12 +4269,12 @@
       <c r="AB29" s="49"/>
       <c r="AC29" s="50"/>
       <c r="AD29" s="51"/>
-      <c r="AE29" s="198"/>
-      <c r="AF29" s="199"/>
-      <c r="AG29" s="199"/>
-      <c r="AH29" s="199"/>
-      <c r="AI29" s="199"/>
-      <c r="AJ29" s="197"/>
+      <c r="AE29" s="159"/>
+      <c r="AF29" s="160"/>
+      <c r="AG29" s="160"/>
+      <c r="AH29" s="160"/>
+      <c r="AI29" s="160"/>
+      <c r="AJ29" s="161"/>
     </row>
     <row r="30" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18">
@@ -4306,12 +4309,12 @@
       <c r="AB30" s="49"/>
       <c r="AC30" s="50"/>
       <c r="AD30" s="51"/>
-      <c r="AE30" s="198"/>
-      <c r="AF30" s="199"/>
-      <c r="AG30" s="199"/>
-      <c r="AH30" s="199"/>
-      <c r="AI30" s="199"/>
-      <c r="AJ30" s="197"/>
+      <c r="AE30" s="159"/>
+      <c r="AF30" s="160"/>
+      <c r="AG30" s="160"/>
+      <c r="AH30" s="160"/>
+      <c r="AI30" s="160"/>
+      <c r="AJ30" s="161"/>
     </row>
     <row r="31" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="31">
@@ -4346,12 +4349,12 @@
       <c r="AB31" s="49"/>
       <c r="AC31" s="50"/>
       <c r="AD31" s="51"/>
-      <c r="AE31" s="198"/>
-      <c r="AF31" s="199"/>
-      <c r="AG31" s="199"/>
-      <c r="AH31" s="199"/>
-      <c r="AI31" s="199"/>
-      <c r="AJ31" s="197"/>
+      <c r="AE31" s="159"/>
+      <c r="AF31" s="160"/>
+      <c r="AG31" s="160"/>
+      <c r="AH31" s="160"/>
+      <c r="AI31" s="160"/>
+      <c r="AJ31" s="161"/>
     </row>
     <row r="32" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18">
@@ -4386,12 +4389,12 @@
       <c r="AB32" s="49"/>
       <c r="AC32" s="50"/>
       <c r="AD32" s="51"/>
-      <c r="AE32" s="198"/>
-      <c r="AF32" s="199"/>
-      <c r="AG32" s="199"/>
-      <c r="AH32" s="199"/>
-      <c r="AI32" s="199"/>
-      <c r="AJ32" s="197"/>
+      <c r="AE32" s="159"/>
+      <c r="AF32" s="160"/>
+      <c r="AG32" s="160"/>
+      <c r="AH32" s="160"/>
+      <c r="AI32" s="160"/>
+      <c r="AJ32" s="161"/>
     </row>
     <row r="33" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="31">
@@ -4426,12 +4429,12 @@
       <c r="AB33" s="49"/>
       <c r="AC33" s="50"/>
       <c r="AD33" s="51"/>
-      <c r="AE33" s="198"/>
-      <c r="AF33" s="199"/>
-      <c r="AG33" s="199"/>
-      <c r="AH33" s="199"/>
-      <c r="AI33" s="199"/>
-      <c r="AJ33" s="197"/>
+      <c r="AE33" s="159"/>
+      <c r="AF33" s="160"/>
+      <c r="AG33" s="160"/>
+      <c r="AH33" s="160"/>
+      <c r="AI33" s="160"/>
+      <c r="AJ33" s="161"/>
     </row>
     <row r="34" spans="1:36" ht="24.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="18">
@@ -4466,12 +4469,12 @@
       <c r="AB34" s="56"/>
       <c r="AC34" s="57"/>
       <c r="AD34" s="58"/>
-      <c r="AE34" s="187"/>
-      <c r="AF34" s="188"/>
-      <c r="AG34" s="188"/>
-      <c r="AH34" s="188"/>
-      <c r="AI34" s="188"/>
-      <c r="AJ34" s="189"/>
+      <c r="AE34" s="167"/>
+      <c r="AF34" s="168"/>
+      <c r="AG34" s="168"/>
+      <c r="AH34" s="168"/>
+      <c r="AI34" s="168"/>
+      <c r="AJ34" s="169"/>
     </row>
     <row r="35" spans="1:36" ht="24.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A35" s="31">
@@ -4506,12 +4509,12 @@
       <c r="AB35" s="27"/>
       <c r="AC35" s="29"/>
       <c r="AD35" s="30"/>
-      <c r="AE35" s="200"/>
-      <c r="AF35" s="201"/>
-      <c r="AG35" s="201"/>
-      <c r="AH35" s="201"/>
-      <c r="AI35" s="201"/>
-      <c r="AJ35" s="202"/>
+      <c r="AE35" s="164"/>
+      <c r="AF35" s="165"/>
+      <c r="AG35" s="165"/>
+      <c r="AH35" s="165"/>
+      <c r="AI35" s="165"/>
+      <c r="AJ35" s="166"/>
     </row>
     <row r="36" spans="1:36" ht="24.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="18">
@@ -5186,12 +5189,12 @@
       <c r="AB52" s="27"/>
       <c r="AC52" s="29"/>
       <c r="AD52" s="30"/>
-      <c r="AE52" s="198"/>
-      <c r="AF52" s="199"/>
-      <c r="AG52" s="199"/>
-      <c r="AH52" s="199"/>
-      <c r="AI52" s="199"/>
-      <c r="AJ52" s="197"/>
+      <c r="AE52" s="159"/>
+      <c r="AF52" s="160"/>
+      <c r="AG52" s="160"/>
+      <c r="AH52" s="160"/>
+      <c r="AI52" s="160"/>
+      <c r="AJ52" s="161"/>
     </row>
     <row r="53" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="31">
@@ -5226,12 +5229,12 @@
       <c r="AB53" s="27"/>
       <c r="AC53" s="29"/>
       <c r="AD53" s="30"/>
-      <c r="AE53" s="198"/>
-      <c r="AF53" s="199"/>
-      <c r="AG53" s="199"/>
-      <c r="AH53" s="199"/>
-      <c r="AI53" s="199"/>
-      <c r="AJ53" s="197"/>
+      <c r="AE53" s="159"/>
+      <c r="AF53" s="160"/>
+      <c r="AG53" s="160"/>
+      <c r="AH53" s="160"/>
+      <c r="AI53" s="160"/>
+      <c r="AJ53" s="161"/>
     </row>
     <row r="54" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="31">
@@ -5266,12 +5269,12 @@
       <c r="AB54" s="27"/>
       <c r="AC54" s="29"/>
       <c r="AD54" s="30"/>
-      <c r="AE54" s="198"/>
-      <c r="AF54" s="199"/>
-      <c r="AG54" s="199"/>
-      <c r="AH54" s="199"/>
-      <c r="AI54" s="199"/>
-      <c r="AJ54" s="197"/>
+      <c r="AE54" s="159"/>
+      <c r="AF54" s="160"/>
+      <c r="AG54" s="160"/>
+      <c r="AH54" s="160"/>
+      <c r="AI54" s="160"/>
+      <c r="AJ54" s="161"/>
     </row>
     <row r="55" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="31">
@@ -5306,12 +5309,12 @@
       <c r="AB55" s="27"/>
       <c r="AC55" s="29"/>
       <c r="AD55" s="30"/>
-      <c r="AE55" s="198"/>
-      <c r="AF55" s="199"/>
-      <c r="AG55" s="199"/>
-      <c r="AH55" s="199"/>
-      <c r="AI55" s="199"/>
-      <c r="AJ55" s="197"/>
+      <c r="AE55" s="159"/>
+      <c r="AF55" s="160"/>
+      <c r="AG55" s="160"/>
+      <c r="AH55" s="160"/>
+      <c r="AI55" s="160"/>
+      <c r="AJ55" s="161"/>
     </row>
     <row r="56" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="31">
@@ -5346,12 +5349,12 @@
       <c r="AB56" s="27"/>
       <c r="AC56" s="29"/>
       <c r="AD56" s="30"/>
-      <c r="AE56" s="198"/>
-      <c r="AF56" s="199"/>
-      <c r="AG56" s="199"/>
-      <c r="AH56" s="199"/>
-      <c r="AI56" s="199"/>
-      <c r="AJ56" s="197"/>
+      <c r="AE56" s="159"/>
+      <c r="AF56" s="160"/>
+      <c r="AG56" s="160"/>
+      <c r="AH56" s="160"/>
+      <c r="AI56" s="160"/>
+      <c r="AJ56" s="161"/>
     </row>
     <row r="57" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="31">
@@ -5386,12 +5389,12 @@
       <c r="AB57" s="27"/>
       <c r="AC57" s="29"/>
       <c r="AD57" s="30"/>
-      <c r="AE57" s="198"/>
-      <c r="AF57" s="199"/>
-      <c r="AG57" s="199"/>
-      <c r="AH57" s="199"/>
-      <c r="AI57" s="199"/>
-      <c r="AJ57" s="197"/>
+      <c r="AE57" s="159"/>
+      <c r="AF57" s="160"/>
+      <c r="AG57" s="160"/>
+      <c r="AH57" s="160"/>
+      <c r="AI57" s="160"/>
+      <c r="AJ57" s="161"/>
     </row>
     <row r="58" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="31">
@@ -5426,12 +5429,12 @@
       <c r="AB58" s="27"/>
       <c r="AC58" s="29"/>
       <c r="AD58" s="30"/>
-      <c r="AE58" s="198"/>
-      <c r="AF58" s="199"/>
-      <c r="AG58" s="199"/>
-      <c r="AH58" s="199"/>
-      <c r="AI58" s="199"/>
-      <c r="AJ58" s="197"/>
+      <c r="AE58" s="159"/>
+      <c r="AF58" s="160"/>
+      <c r="AG58" s="160"/>
+      <c r="AH58" s="160"/>
+      <c r="AI58" s="160"/>
+      <c r="AJ58" s="161"/>
     </row>
     <row r="59" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="31">
@@ -5466,12 +5469,12 @@
       <c r="AB59" s="27"/>
       <c r="AC59" s="29"/>
       <c r="AD59" s="30"/>
-      <c r="AE59" s="198"/>
-      <c r="AF59" s="199"/>
-      <c r="AG59" s="199"/>
-      <c r="AH59" s="199"/>
-      <c r="AI59" s="199"/>
-      <c r="AJ59" s="197"/>
+      <c r="AE59" s="159"/>
+      <c r="AF59" s="160"/>
+      <c r="AG59" s="160"/>
+      <c r="AH59" s="160"/>
+      <c r="AI59" s="160"/>
+      <c r="AJ59" s="161"/>
     </row>
     <row r="60" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="31">
@@ -5506,12 +5509,12 @@
       <c r="AB60" s="27"/>
       <c r="AC60" s="29"/>
       <c r="AD60" s="30"/>
-      <c r="AE60" s="198"/>
-      <c r="AF60" s="199"/>
-      <c r="AG60" s="199"/>
-      <c r="AH60" s="199"/>
-      <c r="AI60" s="199"/>
-      <c r="AJ60" s="197"/>
+      <c r="AE60" s="159"/>
+      <c r="AF60" s="160"/>
+      <c r="AG60" s="160"/>
+      <c r="AH60" s="160"/>
+      <c r="AI60" s="160"/>
+      <c r="AJ60" s="161"/>
     </row>
     <row r="61" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="31">
@@ -5546,12 +5549,12 @@
       <c r="AB61" s="27"/>
       <c r="AC61" s="29"/>
       <c r="AD61" s="30"/>
-      <c r="AE61" s="198"/>
-      <c r="AF61" s="199"/>
-      <c r="AG61" s="199"/>
-      <c r="AH61" s="199"/>
-      <c r="AI61" s="199"/>
-      <c r="AJ61" s="197"/>
+      <c r="AE61" s="159"/>
+      <c r="AF61" s="160"/>
+      <c r="AG61" s="160"/>
+      <c r="AH61" s="160"/>
+      <c r="AI61" s="160"/>
+      <c r="AJ61" s="161"/>
     </row>
     <row r="62" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="31">
@@ -5586,12 +5589,12 @@
       <c r="AB62" s="27"/>
       <c r="AC62" s="29"/>
       <c r="AD62" s="30"/>
-      <c r="AE62" s="198"/>
-      <c r="AF62" s="199"/>
-      <c r="AG62" s="199"/>
-      <c r="AH62" s="199"/>
-      <c r="AI62" s="199"/>
-      <c r="AJ62" s="197"/>
+      <c r="AE62" s="159"/>
+      <c r="AF62" s="160"/>
+      <c r="AG62" s="160"/>
+      <c r="AH62" s="160"/>
+      <c r="AI62" s="160"/>
+      <c r="AJ62" s="161"/>
     </row>
     <row r="63" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="31">
@@ -5626,17 +5629,17 @@
       <c r="AB63" s="27"/>
       <c r="AC63" s="29"/>
       <c r="AD63" s="30"/>
-      <c r="AE63" s="198"/>
-      <c r="AF63" s="199"/>
-      <c r="AG63" s="199"/>
-      <c r="AH63" s="199"/>
-      <c r="AI63" s="199"/>
-      <c r="AJ63" s="197"/>
+      <c r="AE63" s="159"/>
+      <c r="AF63" s="160"/>
+      <c r="AG63" s="160"/>
+      <c r="AH63" s="160"/>
+      <c r="AI63" s="160"/>
+      <c r="AJ63" s="161"/>
     </row>
     <row r="64" spans="1:36" ht="21.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="31"/>
-      <c r="B64" s="196"/>
-      <c r="C64" s="197"/>
+      <c r="B64" s="173"/>
+      <c r="C64" s="161"/>
       <c r="D64" s="65"/>
       <c r="E64" s="34"/>
       <c r="F64" s="34"/>
@@ -5664,17 +5667,17 @@
       <c r="AB64" s="38"/>
       <c r="AC64" s="40"/>
       <c r="AD64" s="41"/>
-      <c r="AE64" s="198"/>
-      <c r="AF64" s="199"/>
-      <c r="AG64" s="199"/>
-      <c r="AH64" s="199"/>
-      <c r="AI64" s="199"/>
-      <c r="AJ64" s="197"/>
+      <c r="AE64" s="159"/>
+      <c r="AF64" s="160"/>
+      <c r="AG64" s="160"/>
+      <c r="AH64" s="160"/>
+      <c r="AI64" s="160"/>
+      <c r="AJ64" s="161"/>
     </row>
     <row r="65" spans="1:37" ht="21.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="31"/>
-      <c r="B65" s="196"/>
-      <c r="C65" s="197"/>
+      <c r="B65" s="173"/>
+      <c r="C65" s="161"/>
       <c r="D65" s="39"/>
       <c r="E65" s="37"/>
       <c r="F65" s="37"/>
@@ -5702,17 +5705,17 @@
       <c r="AB65" s="38"/>
       <c r="AC65" s="40"/>
       <c r="AD65" s="41"/>
-      <c r="AE65" s="198"/>
-      <c r="AF65" s="199"/>
-      <c r="AG65" s="199"/>
-      <c r="AH65" s="199"/>
-      <c r="AI65" s="199"/>
-      <c r="AJ65" s="197"/>
+      <c r="AE65" s="159"/>
+      <c r="AF65" s="160"/>
+      <c r="AG65" s="160"/>
+      <c r="AH65" s="160"/>
+      <c r="AI65" s="160"/>
+      <c r="AJ65" s="161"/>
     </row>
     <row r="66" spans="1:37" ht="21.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="31"/>
-      <c r="B66" s="196"/>
-      <c r="C66" s="197"/>
+      <c r="B66" s="173"/>
+      <c r="C66" s="161"/>
       <c r="D66" s="39"/>
       <c r="E66" s="37"/>
       <c r="F66" s="37"/>
@@ -5740,17 +5743,17 @@
       <c r="AB66" s="38"/>
       <c r="AC66" s="40"/>
       <c r="AD66" s="41"/>
-      <c r="AE66" s="198"/>
-      <c r="AF66" s="199"/>
-      <c r="AG66" s="199"/>
-      <c r="AH66" s="199"/>
-      <c r="AI66" s="199"/>
-      <c r="AJ66" s="197"/>
+      <c r="AE66" s="159"/>
+      <c r="AF66" s="160"/>
+      <c r="AG66" s="160"/>
+      <c r="AH66" s="160"/>
+      <c r="AI66" s="160"/>
+      <c r="AJ66" s="161"/>
     </row>
     <row r="67" spans="1:37" ht="21.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="31"/>
-      <c r="B67" s="196"/>
-      <c r="C67" s="197"/>
+      <c r="B67" s="173"/>
+      <c r="C67" s="161"/>
       <c r="D67" s="39"/>
       <c r="E67" s="37"/>
       <c r="F67" s="37"/>
@@ -5778,17 +5781,17 @@
       <c r="AB67" s="38"/>
       <c r="AC67" s="40"/>
       <c r="AD67" s="41"/>
-      <c r="AE67" s="198"/>
-      <c r="AF67" s="199"/>
-      <c r="AG67" s="199"/>
-      <c r="AH67" s="199"/>
-      <c r="AI67" s="199"/>
-      <c r="AJ67" s="197"/>
+      <c r="AE67" s="159"/>
+      <c r="AF67" s="160"/>
+      <c r="AG67" s="160"/>
+      <c r="AH67" s="160"/>
+      <c r="AI67" s="160"/>
+      <c r="AJ67" s="161"/>
     </row>
     <row r="68" spans="1:37" ht="21.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="31"/>
-      <c r="B68" s="196"/>
-      <c r="C68" s="197"/>
+      <c r="B68" s="173"/>
+      <c r="C68" s="161"/>
       <c r="D68" s="39"/>
       <c r="E68" s="37"/>
       <c r="F68" s="37"/>
@@ -5816,17 +5819,17 @@
       <c r="AB68" s="38"/>
       <c r="AC68" s="40"/>
       <c r="AD68" s="41"/>
-      <c r="AE68" s="198"/>
-      <c r="AF68" s="199"/>
-      <c r="AG68" s="199"/>
-      <c r="AH68" s="199"/>
-      <c r="AI68" s="199"/>
-      <c r="AJ68" s="197"/>
+      <c r="AE68" s="159"/>
+      <c r="AF68" s="160"/>
+      <c r="AG68" s="160"/>
+      <c r="AH68" s="160"/>
+      <c r="AI68" s="160"/>
+      <c r="AJ68" s="161"/>
     </row>
     <row r="69" spans="1:37" ht="21.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="31"/>
-      <c r="B69" s="196"/>
-      <c r="C69" s="197"/>
+      <c r="B69" s="173"/>
+      <c r="C69" s="161"/>
       <c r="D69" s="39"/>
       <c r="E69" s="37"/>
       <c r="F69" s="37"/>
@@ -5854,17 +5857,17 @@
       <c r="AB69" s="38"/>
       <c r="AC69" s="40"/>
       <c r="AD69" s="41"/>
-      <c r="AE69" s="198"/>
-      <c r="AF69" s="199"/>
-      <c r="AG69" s="199"/>
-      <c r="AH69" s="199"/>
-      <c r="AI69" s="199"/>
-      <c r="AJ69" s="197"/>
+      <c r="AE69" s="159"/>
+      <c r="AF69" s="160"/>
+      <c r="AG69" s="160"/>
+      <c r="AH69" s="160"/>
+      <c r="AI69" s="160"/>
+      <c r="AJ69" s="161"/>
     </row>
     <row r="70" spans="1:37" ht="21.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="31"/>
-      <c r="B70" s="196"/>
-      <c r="C70" s="197"/>
+      <c r="B70" s="173"/>
+      <c r="C70" s="161"/>
       <c r="D70" s="39"/>
       <c r="E70" s="37"/>
       <c r="F70" s="37"/>
@@ -5892,17 +5895,17 @@
       <c r="AB70" s="38"/>
       <c r="AC70" s="40"/>
       <c r="AD70" s="41"/>
-      <c r="AE70" s="198"/>
-      <c r="AF70" s="199"/>
-      <c r="AG70" s="199"/>
-      <c r="AH70" s="199"/>
-      <c r="AI70" s="199"/>
-      <c r="AJ70" s="197"/>
+      <c r="AE70" s="159"/>
+      <c r="AF70" s="160"/>
+      <c r="AG70" s="160"/>
+      <c r="AH70" s="160"/>
+      <c r="AI70" s="160"/>
+      <c r="AJ70" s="161"/>
     </row>
     <row r="71" spans="1:37" ht="21.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="31"/>
-      <c r="B71" s="196"/>
-      <c r="C71" s="197"/>
+      <c r="B71" s="173"/>
+      <c r="C71" s="161"/>
       <c r="D71" s="39"/>
       <c r="E71" s="37"/>
       <c r="F71" s="37"/>
@@ -5930,17 +5933,17 @@
       <c r="AB71" s="38"/>
       <c r="AC71" s="40"/>
       <c r="AD71" s="41"/>
-      <c r="AE71" s="198"/>
-      <c r="AF71" s="199"/>
-      <c r="AG71" s="199"/>
-      <c r="AH71" s="199"/>
-      <c r="AI71" s="199"/>
-      <c r="AJ71" s="197"/>
+      <c r="AE71" s="159"/>
+      <c r="AF71" s="160"/>
+      <c r="AG71" s="160"/>
+      <c r="AH71" s="160"/>
+      <c r="AI71" s="160"/>
+      <c r="AJ71" s="161"/>
     </row>
     <row r="72" spans="1:37" ht="21.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="31"/>
-      <c r="B72" s="196"/>
-      <c r="C72" s="197"/>
+      <c r="B72" s="173"/>
+      <c r="C72" s="161"/>
       <c r="D72" s="39"/>
       <c r="E72" s="37"/>
       <c r="F72" s="37"/>
@@ -5968,17 +5971,17 @@
       <c r="AB72" s="38"/>
       <c r="AC72" s="40"/>
       <c r="AD72" s="41"/>
-      <c r="AE72" s="198"/>
-      <c r="AF72" s="199"/>
-      <c r="AG72" s="199"/>
-      <c r="AH72" s="199"/>
-      <c r="AI72" s="199"/>
-      <c r="AJ72" s="197"/>
+      <c r="AE72" s="159"/>
+      <c r="AF72" s="160"/>
+      <c r="AG72" s="160"/>
+      <c r="AH72" s="160"/>
+      <c r="AI72" s="160"/>
+      <c r="AJ72" s="161"/>
     </row>
     <row r="73" spans="1:37" ht="21.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="31"/>
-      <c r="B73" s="196"/>
-      <c r="C73" s="197"/>
+      <c r="B73" s="173"/>
+      <c r="C73" s="161"/>
       <c r="D73" s="39"/>
       <c r="E73" s="37"/>
       <c r="F73" s="37"/>
@@ -6006,17 +6009,17 @@
       <c r="AB73" s="38"/>
       <c r="AC73" s="40"/>
       <c r="AD73" s="41"/>
-      <c r="AE73" s="198"/>
-      <c r="AF73" s="199"/>
-      <c r="AG73" s="199"/>
-      <c r="AH73" s="199"/>
-      <c r="AI73" s="199"/>
-      <c r="AJ73" s="197"/>
+      <c r="AE73" s="159"/>
+      <c r="AF73" s="160"/>
+      <c r="AG73" s="160"/>
+      <c r="AH73" s="160"/>
+      <c r="AI73" s="160"/>
+      <c r="AJ73" s="161"/>
     </row>
     <row r="74" spans="1:37" ht="21.9" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="67"/>
-      <c r="B74" s="185"/>
-      <c r="C74" s="186"/>
+      <c r="B74" s="174"/>
+      <c r="C74" s="175"/>
       <c r="D74" s="52"/>
       <c r="E74" s="53"/>
       <c r="F74" s="53"/>
@@ -6044,19 +6047,19 @@
       <c r="AB74" s="56"/>
       <c r="AC74" s="57"/>
       <c r="AD74" s="58"/>
-      <c r="AE74" s="187"/>
-      <c r="AF74" s="188"/>
-      <c r="AG74" s="188"/>
-      <c r="AH74" s="188"/>
-      <c r="AI74" s="188"/>
-      <c r="AJ74" s="189"/>
+      <c r="AE74" s="167"/>
+      <c r="AF74" s="168"/>
+      <c r="AG74" s="168"/>
+      <c r="AH74" s="168"/>
+      <c r="AI74" s="168"/>
+      <c r="AJ74" s="169"/>
     </row>
     <row r="75" spans="1:37" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="190" t="s">
+      <c r="A75" s="176" t="s">
         <v>20</v>
       </c>
-      <c r="B75" s="190"/>
-      <c r="C75" s="190"/>
+      <c r="B75" s="176"/>
+      <c r="C75" s="176"/>
       <c r="D75" s="68">
         <f>IF(OR(ISBLANK(D11), NOT(ISNUMBER(D11))), 0, $AJ$79 - COUNTIF(D14:D63, "X"))</f>
         <v>0</v>
@@ -6159,26 +6162,26 @@
       </c>
       <c r="AC75" s="69"/>
       <c r="AD75" s="70"/>
-      <c r="AE75" s="191"/>
-      <c r="AF75" s="192"/>
-      <c r="AG75" s="192"/>
-      <c r="AH75" s="192"/>
-      <c r="AI75" s="192"/>
-      <c r="AJ75" s="193"/>
+      <c r="AE75" s="177"/>
+      <c r="AF75" s="178"/>
+      <c r="AG75" s="178"/>
+      <c r="AH75" s="178"/>
+      <c r="AI75" s="178"/>
+      <c r="AJ75" s="179"/>
       <c r="AK75" s="5">
         <f>SUM(D75:AB75)</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:37" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="194"/>
-      <c r="B76" s="194"/>
+      <c r="A76" s="180"/>
+      <c r="B76" s="180"/>
       <c r="C76" s="71"/>
-      <c r="D76" s="195"/>
-      <c r="E76" s="195"/>
-      <c r="F76" s="195"/>
-      <c r="G76" s="195"/>
-      <c r="H76" s="195"/>
+      <c r="D76" s="181"/>
+      <c r="E76" s="181"/>
+      <c r="F76" s="181"/>
+      <c r="G76" s="181"/>
+      <c r="H76" s="181"/>
     </row>
     <row r="77" spans="1:37" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="72" t="s">
@@ -6214,55 +6217,55 @@
       <c r="AB77" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="AC77" s="169">
+      <c r="AC77" s="188">
         <f>X6</f>
         <v>0</v>
       </c>
-      <c r="AD77" s="170"/>
-      <c r="AE77" s="171" t="s">
+      <c r="AD77" s="189"/>
+      <c r="AE77" s="190" t="s">
         <v>24</v>
       </c>
-      <c r="AF77" s="172"/>
+      <c r="AF77" s="191"/>
       <c r="AG77" s="82">
         <f>COUNT(D11:AB11)</f>
         <v>0</v>
       </c>
-      <c r="AH77" s="175" t="s">
+      <c r="AH77" s="194" t="s">
         <v>25</v>
       </c>
-      <c r="AI77" s="175"/>
-      <c r="AJ77" s="176"/>
+      <c r="AI77" s="194"/>
+      <c r="AJ77" s="195"/>
     </row>
     <row r="78" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="147" t="s">
+      <c r="A78" s="182" t="s">
         <v>26</v>
       </c>
-      <c r="B78" s="147"/>
-      <c r="C78" s="147"/>
-      <c r="D78" s="147"/>
-      <c r="E78" s="147"/>
-      <c r="F78" s="147"/>
-      <c r="G78" s="147"/>
-      <c r="H78" s="147"/>
-      <c r="I78" s="147"/>
-      <c r="J78" s="147"/>
-      <c r="K78" s="147"/>
-      <c r="L78" s="147"/>
-      <c r="M78" s="147"/>
-      <c r="N78" s="147"/>
+      <c r="B78" s="182"/>
+      <c r="C78" s="182"/>
+      <c r="D78" s="182"/>
+      <c r="E78" s="182"/>
+      <c r="F78" s="182"/>
+      <c r="G78" s="182"/>
+      <c r="H78" s="182"/>
+      <c r="I78" s="182"/>
+      <c r="J78" s="182"/>
+      <c r="K78" s="182"/>
+      <c r="L78" s="182"/>
+      <c r="M78" s="182"/>
+      <c r="N78" s="182"/>
       <c r="O78" s="74"/>
       <c r="P78" s="75"/>
-      <c r="Q78" s="177" t="s">
+      <c r="Q78" s="196" t="s">
         <v>27</v>
       </c>
-      <c r="R78" s="178"/>
-      <c r="S78" s="178"/>
-      <c r="T78" s="178"/>
-      <c r="U78" s="178"/>
-      <c r="V78" s="178"/>
-      <c r="W78" s="178"/>
-      <c r="X78" s="178"/>
-      <c r="Y78" s="178"/>
+      <c r="R78" s="197"/>
+      <c r="S78" s="197"/>
+      <c r="T78" s="197"/>
+      <c r="U78" s="197"/>
+      <c r="V78" s="197"/>
+      <c r="W78" s="197"/>
+      <c r="X78" s="197"/>
+      <c r="Y78" s="197"/>
       <c r="Z78" s="83"/>
       <c r="AB78" s="84"/>
       <c r="AC78" s="85"/>
@@ -6270,8 +6273,8 @@
         <f>COUNT(D11:AB11)</f>
         <v>0</v>
       </c>
-      <c r="AE78" s="173"/>
-      <c r="AF78" s="174"/>
+      <c r="AE78" s="192"/>
+      <c r="AF78" s="193"/>
       <c r="AG78" s="87"/>
       <c r="AH78" s="88"/>
       <c r="AI78" s="89"/>
@@ -6280,109 +6283,109 @@
       </c>
     </row>
     <row r="79" spans="1:37" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A79" s="147" t="s">
+      <c r="A79" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="B79" s="147"/>
-      <c r="C79" s="147"/>
-      <c r="D79" s="147"/>
-      <c r="E79" s="147"/>
-      <c r="F79" s="147"/>
-      <c r="G79" s="147"/>
-      <c r="H79" s="147"/>
-      <c r="I79" s="147"/>
-      <c r="J79" s="147"/>
-      <c r="K79" s="147"/>
-      <c r="L79" s="147"/>
-      <c r="M79" s="147"/>
-      <c r="N79" s="147"/>
+      <c r="B79" s="182"/>
+      <c r="C79" s="182"/>
+      <c r="D79" s="182"/>
+      <c r="E79" s="182"/>
+      <c r="F79" s="182"/>
+      <c r="G79" s="182"/>
+      <c r="H79" s="182"/>
+      <c r="I79" s="182"/>
+      <c r="J79" s="182"/>
+      <c r="K79" s="182"/>
+      <c r="L79" s="182"/>
+      <c r="M79" s="182"/>
+      <c r="N79" s="182"/>
       <c r="O79" s="74"/>
       <c r="P79" s="75"/>
-      <c r="Q79" s="131"/>
-      <c r="R79" s="132"/>
-      <c r="S79" s="132"/>
-      <c r="T79" s="132"/>
-      <c r="U79" s="132"/>
-      <c r="V79" s="132"/>
-      <c r="W79" s="132"/>
-      <c r="X79" s="132"/>
-      <c r="Y79" s="132"/>
+      <c r="Q79" s="198"/>
+      <c r="R79" s="199"/>
+      <c r="S79" s="199"/>
+      <c r="T79" s="199"/>
+      <c r="U79" s="199"/>
+      <c r="V79" s="199"/>
+      <c r="W79" s="199"/>
+      <c r="X79" s="199"/>
+      <c r="Y79" s="199"/>
       <c r="Z79" s="83"/>
-      <c r="AB79" s="179" t="s">
+      <c r="AB79" s="200" t="s">
         <v>30</v>
       </c>
-      <c r="AC79" s="180"/>
-      <c r="AD79" s="180"/>
-      <c r="AE79" s="180"/>
-      <c r="AF79" s="180"/>
-      <c r="AG79" s="181"/>
-      <c r="AH79" s="156"/>
-      <c r="AI79" s="156"/>
-      <c r="AJ79" s="157"/>
+      <c r="AC79" s="201"/>
+      <c r="AD79" s="201"/>
+      <c r="AE79" s="201"/>
+      <c r="AF79" s="201"/>
+      <c r="AG79" s="202"/>
+      <c r="AH79" s="206"/>
+      <c r="AI79" s="206"/>
+      <c r="AJ79" s="208"/>
     </row>
     <row r="80" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="147" t="s">
+      <c r="A80" s="182" t="s">
         <v>31</v>
       </c>
-      <c r="B80" s="147"/>
-      <c r="C80" s="147"/>
-      <c r="D80" s="147"/>
-      <c r="E80" s="147"/>
-      <c r="F80" s="147"/>
-      <c r="G80" s="147"/>
-      <c r="H80" s="147"/>
-      <c r="I80" s="147"/>
-      <c r="J80" s="147"/>
-      <c r="K80" s="147"/>
-      <c r="L80" s="147"/>
-      <c r="M80" s="147"/>
-      <c r="N80" s="147"/>
+      <c r="B80" s="182"/>
+      <c r="C80" s="182"/>
+      <c r="D80" s="182"/>
+      <c r="E80" s="182"/>
+      <c r="F80" s="182"/>
+      <c r="G80" s="182"/>
+      <c r="H80" s="182"/>
+      <c r="I80" s="182"/>
+      <c r="J80" s="182"/>
+      <c r="K80" s="182"/>
+      <c r="L80" s="182"/>
+      <c r="M80" s="182"/>
+      <c r="N80" s="182"/>
       <c r="O80" s="74"/>
       <c r="P80" s="75"/>
-      <c r="Q80" s="131"/>
-      <c r="R80" s="132"/>
-      <c r="S80" s="132"/>
-      <c r="T80" s="132"/>
-      <c r="U80" s="132"/>
-      <c r="V80" s="132"/>
-      <c r="W80" s="132"/>
-      <c r="X80" s="132"/>
-      <c r="Y80" s="132"/>
+      <c r="Q80" s="198"/>
+      <c r="R80" s="199"/>
+      <c r="S80" s="199"/>
+      <c r="T80" s="199"/>
+      <c r="U80" s="199"/>
+      <c r="V80" s="199"/>
+      <c r="W80" s="199"/>
+      <c r="X80" s="199"/>
+      <c r="Y80" s="199"/>
       <c r="Z80" s="83"/>
-      <c r="AB80" s="182"/>
-      <c r="AC80" s="183"/>
-      <c r="AD80" s="183"/>
-      <c r="AE80" s="183"/>
-      <c r="AF80" s="183"/>
-      <c r="AG80" s="184"/>
-      <c r="AH80" s="127"/>
-      <c r="AI80" s="127"/>
-      <c r="AJ80" s="129"/>
+      <c r="AB80" s="203"/>
+      <c r="AC80" s="204"/>
+      <c r="AD80" s="204"/>
+      <c r="AE80" s="204"/>
+      <c r="AF80" s="204"/>
+      <c r="AG80" s="205"/>
+      <c r="AH80" s="207"/>
+      <c r="AI80" s="207"/>
+      <c r="AJ80" s="209"/>
     </row>
     <row r="81" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="153" t="s">
+      <c r="A81" s="183" t="s">
         <v>32</v>
       </c>
-      <c r="B81" s="168" t="s">
+      <c r="B81" s="124" t="s">
         <v>33</v>
       </c>
       <c r="C81" s="91"/>
-      <c r="D81" s="161" t="s">
+      <c r="D81" s="184" t="s">
         <v>34</v>
       </c>
-      <c r="E81" s="161"/>
-      <c r="F81" s="161"/>
-      <c r="G81" s="161"/>
-      <c r="H81" s="161"/>
-      <c r="I81" s="161"/>
-      <c r="J81" s="161"/>
-      <c r="K81" s="161"/>
-      <c r="L81" s="161"/>
-      <c r="M81" s="161"/>
-      <c r="N81" s="146" t="s">
+      <c r="E81" s="184"/>
+      <c r="F81" s="184"/>
+      <c r="G81" s="184"/>
+      <c r="H81" s="184"/>
+      <c r="I81" s="184"/>
+      <c r="J81" s="184"/>
+      <c r="K81" s="184"/>
+      <c r="L81" s="184"/>
+      <c r="M81" s="184"/>
+      <c r="N81" s="185" t="s">
         <v>35</v>
       </c>
-      <c r="O81" s="146"/>
+      <c r="O81" s="185"/>
       <c r="P81" s="75"/>
       <c r="Q81" s="92" t="s">
         <v>36</v>
@@ -6390,38 +6393,38 @@
       <c r="V81" s="2"/>
       <c r="Y81" s="93"/>
       <c r="Z81" s="83"/>
-      <c r="AB81" s="138" t="s">
+      <c r="AB81" s="186" t="s">
         <v>37</v>
       </c>
-      <c r="AC81" s="139"/>
-      <c r="AD81" s="139"/>
-      <c r="AE81" s="139"/>
-      <c r="AF81" s="139"/>
-      <c r="AG81" s="139"/>
-      <c r="AH81" s="134"/>
-      <c r="AI81" s="134"/>
-      <c r="AJ81" s="135">
+      <c r="AC81" s="187"/>
+      <c r="AD81" s="187"/>
+      <c r="AE81" s="187"/>
+      <c r="AF81" s="187"/>
+      <c r="AG81" s="187"/>
+      <c r="AH81" s="210"/>
+      <c r="AI81" s="210"/>
+      <c r="AJ81" s="211">
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="153"/>
-      <c r="B82" s="168"/>
+      <c r="A82" s="183"/>
+      <c r="B82" s="124"/>
       <c r="C82" s="91"/>
-      <c r="D82" s="158" t="s">
+      <c r="D82" s="212" t="s">
         <v>38</v>
       </c>
-      <c r="E82" s="158"/>
-      <c r="F82" s="158"/>
-      <c r="G82" s="158"/>
-      <c r="H82" s="158"/>
-      <c r="I82" s="158"/>
-      <c r="J82" s="158"/>
-      <c r="K82" s="158"/>
-      <c r="L82" s="158"/>
-      <c r="M82" s="158"/>
-      <c r="N82" s="146"/>
-      <c r="O82" s="146"/>
+      <c r="E82" s="212"/>
+      <c r="F82" s="212"/>
+      <c r="G82" s="212"/>
+      <c r="H82" s="212"/>
+      <c r="I82" s="212"/>
+      <c r="J82" s="212"/>
+      <c r="K82" s="212"/>
+      <c r="L82" s="212"/>
+      <c r="M82" s="212"/>
+      <c r="N82" s="185"/>
+      <c r="O82" s="185"/>
       <c r="P82" s="75"/>
       <c r="Q82" s="92" t="s">
         <v>39</v>
@@ -6433,36 +6436,36 @@
       <c r="V82" s="2"/>
       <c r="Y82" s="93"/>
       <c r="Z82" s="83"/>
-      <c r="AB82" s="138"/>
-      <c r="AC82" s="139"/>
-      <c r="AD82" s="139"/>
-      <c r="AE82" s="139"/>
-      <c r="AF82" s="139"/>
-      <c r="AG82" s="139"/>
-      <c r="AH82" s="134"/>
-      <c r="AI82" s="134"/>
-      <c r="AJ82" s="135"/>
+      <c r="AB82" s="186"/>
+      <c r="AC82" s="187"/>
+      <c r="AD82" s="187"/>
+      <c r="AE82" s="187"/>
+      <c r="AF82" s="187"/>
+      <c r="AG82" s="187"/>
+      <c r="AH82" s="210"/>
+      <c r="AI82" s="210"/>
+      <c r="AJ82" s="211"/>
     </row>
     <row r="83" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="153" t="s">
+      <c r="A83" s="183" t="s">
         <v>40</v>
       </c>
-      <c r="B83" s="154" t="s">
+      <c r="B83" s="213" t="s">
         <v>41</v>
       </c>
       <c r="C83" s="94"/>
-      <c r="D83" s="155" t="s">
+      <c r="D83" s="214" t="s">
         <v>42</v>
       </c>
-      <c r="E83" s="155"/>
-      <c r="F83" s="155"/>
-      <c r="G83" s="155"/>
-      <c r="H83" s="155"/>
-      <c r="I83" s="155"/>
-      <c r="J83" s="155"/>
-      <c r="K83" s="155"/>
-      <c r="L83" s="155"/>
-      <c r="M83" s="155"/>
+      <c r="E83" s="214"/>
+      <c r="F83" s="214"/>
+      <c r="G83" s="214"/>
+      <c r="H83" s="214"/>
+      <c r="I83" s="214"/>
+      <c r="J83" s="214"/>
+      <c r="K83" s="214"/>
+      <c r="L83" s="214"/>
+      <c r="M83" s="214"/>
       <c r="N83" s="95"/>
       <c r="O83" s="74"/>
       <c r="P83" s="75"/>
@@ -6476,34 +6479,34 @@
       <c r="V83" s="2"/>
       <c r="Y83" s="93"/>
       <c r="Z83" s="83"/>
-      <c r="AB83" s="138" t="s">
+      <c r="AB83" s="186" t="s">
         <v>44</v>
       </c>
-      <c r="AC83" s="139"/>
-      <c r="AD83" s="139"/>
-      <c r="AE83" s="139"/>
-      <c r="AF83" s="139"/>
-      <c r="AG83" s="139"/>
-      <c r="AH83" s="156"/>
-      <c r="AI83" s="156"/>
-      <c r="AJ83" s="157"/>
+      <c r="AC83" s="187"/>
+      <c r="AD83" s="187"/>
+      <c r="AE83" s="187"/>
+      <c r="AF83" s="187"/>
+      <c r="AG83" s="187"/>
+      <c r="AH83" s="206"/>
+      <c r="AI83" s="206"/>
+      <c r="AJ83" s="208"/>
     </row>
     <row r="84" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="153"/>
-      <c r="B84" s="154"/>
+      <c r="A84" s="183"/>
+      <c r="B84" s="213"/>
       <c r="C84" s="94"/>
-      <c r="D84" s="158" t="s">
+      <c r="D84" s="212" t="s">
         <v>45</v>
       </c>
-      <c r="E84" s="158"/>
-      <c r="F84" s="158"/>
-      <c r="G84" s="158"/>
-      <c r="H84" s="158"/>
-      <c r="I84" s="158"/>
-      <c r="J84" s="158"/>
-      <c r="K84" s="158"/>
-      <c r="L84" s="158"/>
-      <c r="M84" s="158"/>
+      <c r="E84" s="212"/>
+      <c r="F84" s="212"/>
+      <c r="G84" s="212"/>
+      <c r="H84" s="212"/>
+      <c r="I84" s="212"/>
+      <c r="J84" s="212"/>
+      <c r="K84" s="212"/>
+      <c r="L84" s="212"/>
+      <c r="M84" s="212"/>
       <c r="N84" s="74"/>
       <c r="O84" s="74"/>
       <c r="P84" s="75"/>
@@ -6513,108 +6516,108 @@
       <c r="V84" s="2"/>
       <c r="Y84" s="93"/>
       <c r="Z84" s="83"/>
-      <c r="AB84" s="138"/>
-      <c r="AC84" s="139"/>
-      <c r="AD84" s="139"/>
-      <c r="AE84" s="139"/>
-      <c r="AF84" s="139"/>
-      <c r="AG84" s="139"/>
-      <c r="AH84" s="127"/>
-      <c r="AI84" s="127"/>
-      <c r="AJ84" s="129"/>
+      <c r="AB84" s="186"/>
+      <c r="AC84" s="187"/>
+      <c r="AD84" s="187"/>
+      <c r="AE84" s="187"/>
+      <c r="AF84" s="187"/>
+      <c r="AG84" s="187"/>
+      <c r="AH84" s="207"/>
+      <c r="AI84" s="207"/>
+      <c r="AJ84" s="209"/>
     </row>
     <row r="85" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="159" t="s">
+      <c r="A85" s="215" t="s">
         <v>47</v>
       </c>
-      <c r="B85" s="160" t="s">
+      <c r="B85" s="216" t="s">
         <v>48</v>
       </c>
-      <c r="C85" s="160"/>
-      <c r="D85" s="161" t="s">
+      <c r="C85" s="216"/>
+      <c r="D85" s="184" t="s">
         <v>49</v>
       </c>
-      <c r="E85" s="161"/>
-      <c r="F85" s="161"/>
-      <c r="G85" s="161"/>
-      <c r="H85" s="161"/>
-      <c r="I85" s="161"/>
-      <c r="J85" s="161"/>
-      <c r="K85" s="161"/>
-      <c r="L85" s="161"/>
-      <c r="M85" s="161"/>
-      <c r="N85" s="146" t="s">
+      <c r="E85" s="184"/>
+      <c r="F85" s="184"/>
+      <c r="G85" s="184"/>
+      <c r="H85" s="184"/>
+      <c r="I85" s="184"/>
+      <c r="J85" s="184"/>
+      <c r="K85" s="184"/>
+      <c r="L85" s="184"/>
+      <c r="M85" s="184"/>
+      <c r="N85" s="185" t="s">
         <v>35</v>
       </c>
-      <c r="O85" s="146"/>
+      <c r="O85" s="185"/>
       <c r="P85" s="75"/>
       <c r="Q85" s="96" t="s">
         <v>50</v>
       </c>
       <c r="Y85" s="93"/>
       <c r="Z85" s="83"/>
-      <c r="AB85" s="162" t="s">
+      <c r="AB85" s="217" t="s">
         <v>51</v>
       </c>
-      <c r="AC85" s="163"/>
-      <c r="AD85" s="163"/>
-      <c r="AE85" s="163"/>
-      <c r="AF85" s="163"/>
-      <c r="AG85" s="163"/>
-      <c r="AH85" s="164"/>
-      <c r="AI85" s="164"/>
-      <c r="AJ85" s="166" t="e">
+      <c r="AC85" s="218"/>
+      <c r="AD85" s="218"/>
+      <c r="AE85" s="218"/>
+      <c r="AF85" s="218"/>
+      <c r="AG85" s="218"/>
+      <c r="AH85" s="219"/>
+      <c r="AI85" s="219"/>
+      <c r="AJ85" s="221" t="e">
         <f>AJ79/AJ83*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="86" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="159"/>
-      <c r="B86" s="160"/>
-      <c r="C86" s="160"/>
-      <c r="D86" s="146" t="s">
+      <c r="A86" s="215"/>
+      <c r="B86" s="216"/>
+      <c r="C86" s="216"/>
+      <c r="D86" s="185" t="s">
         <v>52</v>
       </c>
-      <c r="E86" s="146"/>
-      <c r="F86" s="146"/>
-      <c r="G86" s="146"/>
-      <c r="H86" s="146"/>
-      <c r="I86" s="146"/>
-      <c r="J86" s="146"/>
-      <c r="K86" s="146"/>
-      <c r="L86" s="146"/>
-      <c r="M86" s="146"/>
-      <c r="N86" s="146"/>
-      <c r="O86" s="146"/>
+      <c r="E86" s="185"/>
+      <c r="F86" s="185"/>
+      <c r="G86" s="185"/>
+      <c r="H86" s="185"/>
+      <c r="I86" s="185"/>
+      <c r="J86" s="185"/>
+      <c r="K86" s="185"/>
+      <c r="L86" s="185"/>
+      <c r="M86" s="185"/>
+      <c r="N86" s="185"/>
+      <c r="O86" s="185"/>
       <c r="P86" s="75"/>
       <c r="Q86" s="96" t="s">
         <v>53</v>
       </c>
       <c r="Y86" s="93"/>
       <c r="Z86" s="83"/>
-      <c r="AB86" s="162"/>
-      <c r="AC86" s="163"/>
-      <c r="AD86" s="163"/>
-      <c r="AE86" s="163"/>
-      <c r="AF86" s="163"/>
-      <c r="AG86" s="163"/>
-      <c r="AH86" s="165"/>
-      <c r="AI86" s="165"/>
-      <c r="AJ86" s="167"/>
+      <c r="AB86" s="217"/>
+      <c r="AC86" s="218"/>
+      <c r="AD86" s="218"/>
+      <c r="AE86" s="218"/>
+      <c r="AF86" s="218"/>
+      <c r="AG86" s="218"/>
+      <c r="AH86" s="220"/>
+      <c r="AI86" s="220"/>
+      <c r="AJ86" s="222"/>
     </row>
     <row r="87" spans="1:36" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="147"/>
-      <c r="B87" s="147"/>
-      <c r="C87" s="147"/>
-      <c r="D87" s="147"/>
-      <c r="E87" s="147"/>
-      <c r="F87" s="147"/>
-      <c r="G87" s="147"/>
-      <c r="H87" s="147"/>
-      <c r="I87" s="147"/>
-      <c r="J87" s="147"/>
-      <c r="K87" s="147"/>
-      <c r="L87" s="147"/>
+      <c r="A87" s="182"/>
+      <c r="B87" s="182"/>
+      <c r="C87" s="182"/>
+      <c r="D87" s="182"/>
+      <c r="E87" s="182"/>
+      <c r="F87" s="182"/>
+      <c r="G87" s="182"/>
+      <c r="H87" s="182"/>
+      <c r="I87" s="182"/>
+      <c r="J87" s="182"/>
+      <c r="K87" s="182"/>
+      <c r="L87" s="182"/>
       <c r="M87" s="97"/>
       <c r="N87" s="97"/>
       <c r="O87" s="74"/>
@@ -6624,14 +6627,14 @@
       </c>
       <c r="Y87" s="2"/>
       <c r="Z87" s="83"/>
-      <c r="AB87" s="148" t="s">
+      <c r="AB87" s="231" t="s">
         <v>55</v>
       </c>
-      <c r="AC87" s="149"/>
-      <c r="AD87" s="149"/>
-      <c r="AE87" s="149"/>
-      <c r="AF87" s="149"/>
-      <c r="AG87" s="149"/>
+      <c r="AC87" s="232"/>
+      <c r="AD87" s="232"/>
+      <c r="AE87" s="232"/>
+      <c r="AF87" s="232"/>
+      <c r="AG87" s="232"/>
       <c r="AH87" s="98"/>
       <c r="AI87" s="98"/>
       <c r="AJ87" s="99" t="e">
@@ -6640,22 +6643,22 @@
       </c>
     </row>
     <row r="88" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="150" t="s">
+      <c r="A88" s="233" t="s">
         <v>56</v>
       </c>
-      <c r="B88" s="150"/>
-      <c r="C88" s="150"/>
-      <c r="D88" s="150"/>
-      <c r="E88" s="150"/>
-      <c r="F88" s="150"/>
-      <c r="G88" s="150"/>
-      <c r="H88" s="150"/>
-      <c r="I88" s="150"/>
-      <c r="J88" s="150"/>
-      <c r="K88" s="150"/>
-      <c r="L88" s="150"/>
-      <c r="M88" s="150"/>
-      <c r="N88" s="150"/>
+      <c r="B88" s="233"/>
+      <c r="C88" s="233"/>
+      <c r="D88" s="233"/>
+      <c r="E88" s="233"/>
+      <c r="F88" s="233"/>
+      <c r="G88" s="233"/>
+      <c r="H88" s="233"/>
+      <c r="I88" s="233"/>
+      <c r="J88" s="233"/>
+      <c r="K88" s="233"/>
+      <c r="L88" s="233"/>
+      <c r="M88" s="233"/>
+      <c r="N88" s="233"/>
       <c r="O88" s="95"/>
       <c r="P88" s="75"/>
       <c r="Q88" s="96" t="s">
@@ -6663,36 +6666,36 @@
       </c>
       <c r="Y88" s="93"/>
       <c r="Z88" s="83"/>
-      <c r="AB88" s="138" t="s">
+      <c r="AB88" s="186" t="s">
         <v>58</v>
       </c>
-      <c r="AC88" s="139"/>
-      <c r="AD88" s="139"/>
-      <c r="AE88" s="139"/>
-      <c r="AF88" s="139"/>
-      <c r="AG88" s="139"/>
-      <c r="AH88" s="151"/>
-      <c r="AI88" s="127"/>
-      <c r="AJ88" s="137" t="e">
+      <c r="AC88" s="187"/>
+      <c r="AD88" s="187"/>
+      <c r="AE88" s="187"/>
+      <c r="AF88" s="187"/>
+      <c r="AG88" s="187"/>
+      <c r="AH88" s="234"/>
+      <c r="AI88" s="207"/>
+      <c r="AJ88" s="223" t="e">
         <f>AJ87/AJ83*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="89" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="150"/>
-      <c r="B89" s="150"/>
-      <c r="C89" s="150"/>
-      <c r="D89" s="150"/>
-      <c r="E89" s="150"/>
-      <c r="F89" s="150"/>
-      <c r="G89" s="150"/>
-      <c r="H89" s="150"/>
-      <c r="I89" s="150"/>
-      <c r="J89" s="150"/>
-      <c r="K89" s="150"/>
-      <c r="L89" s="150"/>
-      <c r="M89" s="150"/>
-      <c r="N89" s="150"/>
+      <c r="A89" s="233"/>
+      <c r="B89" s="233"/>
+      <c r="C89" s="233"/>
+      <c r="D89" s="233"/>
+      <c r="E89" s="233"/>
+      <c r="F89" s="233"/>
+      <c r="G89" s="233"/>
+      <c r="H89" s="233"/>
+      <c r="I89" s="233"/>
+      <c r="J89" s="233"/>
+      <c r="K89" s="233"/>
+      <c r="L89" s="233"/>
+      <c r="M89" s="233"/>
+      <c r="N89" s="233"/>
       <c r="O89" s="95"/>
       <c r="P89" s="75"/>
       <c r="Q89" s="96" t="s">
@@ -6700,34 +6703,34 @@
       </c>
       <c r="Y89" s="93"/>
       <c r="Z89" s="83"/>
-      <c r="AB89" s="138"/>
-      <c r="AC89" s="139"/>
-      <c r="AD89" s="139"/>
-      <c r="AE89" s="139"/>
-      <c r="AF89" s="139"/>
-      <c r="AG89" s="139"/>
-      <c r="AH89" s="152"/>
-      <c r="AI89" s="127"/>
-      <c r="AJ89" s="137"/>
+      <c r="AB89" s="186"/>
+      <c r="AC89" s="187"/>
+      <c r="AD89" s="187"/>
+      <c r="AE89" s="187"/>
+      <c r="AF89" s="187"/>
+      <c r="AG89" s="187"/>
+      <c r="AH89" s="235"/>
+      <c r="AI89" s="207"/>
+      <c r="AJ89" s="223"/>
     </row>
     <row r="90" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="136" t="s">
+      <c r="A90" s="224" t="s">
         <v>60</v>
       </c>
-      <c r="B90" s="136"/>
-      <c r="C90" s="136"/>
-      <c r="D90" s="136"/>
-      <c r="E90" s="136"/>
-      <c r="F90" s="136"/>
-      <c r="G90" s="136"/>
-      <c r="H90" s="136"/>
-      <c r="I90" s="136"/>
-      <c r="J90" s="136"/>
-      <c r="K90" s="136"/>
-      <c r="L90" s="136"/>
-      <c r="M90" s="136"/>
-      <c r="N90" s="136"/>
-      <c r="O90" s="136"/>
+      <c r="B90" s="224"/>
+      <c r="C90" s="224"/>
+      <c r="D90" s="224"/>
+      <c r="E90" s="224"/>
+      <c r="F90" s="224"/>
+      <c r="G90" s="224"/>
+      <c r="H90" s="224"/>
+      <c r="I90" s="224"/>
+      <c r="J90" s="224"/>
+      <c r="K90" s="224"/>
+      <c r="L90" s="224"/>
+      <c r="M90" s="224"/>
+      <c r="N90" s="224"/>
+      <c r="O90" s="224"/>
       <c r="P90" s="75"/>
       <c r="Q90" s="96" t="s">
         <v>61</v>
@@ -6735,49 +6738,49 @@
       <c r="Y90" s="93"/>
       <c r="Z90" s="83"/>
       <c r="AA90" s="100"/>
-      <c r="AB90" s="138" t="s">
+      <c r="AB90" s="186" t="s">
         <v>62</v>
       </c>
-      <c r="AC90" s="139"/>
-      <c r="AD90" s="139"/>
-      <c r="AE90" s="139"/>
-      <c r="AF90" s="139"/>
-      <c r="AG90" s="139"/>
-      <c r="AH90" s="140"/>
-      <c r="AI90" s="142"/>
-      <c r="AJ90" s="144"/>
+      <c r="AC90" s="187"/>
+      <c r="AD90" s="187"/>
+      <c r="AE90" s="187"/>
+      <c r="AF90" s="187"/>
+      <c r="AG90" s="187"/>
+      <c r="AH90" s="225"/>
+      <c r="AI90" s="227"/>
+      <c r="AJ90" s="229"/>
     </row>
     <row r="91" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="136"/>
-      <c r="B91" s="136"/>
-      <c r="C91" s="136"/>
-      <c r="D91" s="136"/>
-      <c r="E91" s="136"/>
-      <c r="F91" s="136"/>
-      <c r="G91" s="136"/>
-      <c r="H91" s="136"/>
-      <c r="I91" s="136"/>
-      <c r="J91" s="136"/>
-      <c r="K91" s="136"/>
-      <c r="L91" s="136"/>
-      <c r="M91" s="136"/>
-      <c r="N91" s="136"/>
-      <c r="O91" s="136"/>
+      <c r="A91" s="224"/>
+      <c r="B91" s="224"/>
+      <c r="C91" s="224"/>
+      <c r="D91" s="224"/>
+      <c r="E91" s="224"/>
+      <c r="F91" s="224"/>
+      <c r="G91" s="224"/>
+      <c r="H91" s="224"/>
+      <c r="I91" s="224"/>
+      <c r="J91" s="224"/>
+      <c r="K91" s="224"/>
+      <c r="L91" s="224"/>
+      <c r="M91" s="224"/>
+      <c r="N91" s="224"/>
+      <c r="O91" s="224"/>
       <c r="P91" s="75"/>
       <c r="Q91" s="96" t="s">
         <v>63</v>
       </c>
       <c r="Y91" s="2"/>
       <c r="Z91" s="83"/>
-      <c r="AB91" s="138"/>
-      <c r="AC91" s="139"/>
-      <c r="AD91" s="139"/>
-      <c r="AE91" s="139"/>
-      <c r="AF91" s="139"/>
-      <c r="AG91" s="139"/>
-      <c r="AH91" s="141"/>
-      <c r="AI91" s="143"/>
-      <c r="AJ91" s="145"/>
+      <c r="AB91" s="186"/>
+      <c r="AC91" s="187"/>
+      <c r="AD91" s="187"/>
+      <c r="AE91" s="187"/>
+      <c r="AF91" s="187"/>
+      <c r="AG91" s="187"/>
+      <c r="AH91" s="226"/>
+      <c r="AI91" s="228"/>
+      <c r="AJ91" s="230"/>
     </row>
     <row r="92" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="74" t="s">
@@ -6803,37 +6806,37 @@
       </c>
       <c r="Y92" s="93"/>
       <c r="Z92" s="83"/>
-      <c r="AB92" s="123" t="s">
+      <c r="AB92" s="238" t="s">
         <v>66</v>
       </c>
-      <c r="AC92" s="124"/>
-      <c r="AD92" s="124"/>
-      <c r="AE92" s="124"/>
-      <c r="AF92" s="124"/>
-      <c r="AG92" s="124"/>
-      <c r="AH92" s="134"/>
-      <c r="AI92" s="134"/>
-      <c r="AJ92" s="135"/>
+      <c r="AC92" s="239"/>
+      <c r="AD92" s="239"/>
+      <c r="AE92" s="239"/>
+      <c r="AF92" s="239"/>
+      <c r="AG92" s="239"/>
+      <c r="AH92" s="210"/>
+      <c r="AI92" s="210"/>
+      <c r="AJ92" s="211"/>
     </row>
     <row r="93" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="B93" s="136" t="s">
+      <c r="B93" s="224" t="s">
         <v>68</v>
       </c>
-      <c r="C93" s="136"/>
-      <c r="D93" s="136"/>
-      <c r="E93" s="136"/>
-      <c r="F93" s="136"/>
-      <c r="G93" s="136"/>
-      <c r="H93" s="136"/>
-      <c r="I93" s="136"/>
-      <c r="J93" s="136"/>
-      <c r="K93" s="136"/>
-      <c r="L93" s="136"/>
-      <c r="M93" s="136"/>
-      <c r="N93" s="136"/>
+      <c r="C93" s="224"/>
+      <c r="D93" s="224"/>
+      <c r="E93" s="224"/>
+      <c r="F93" s="224"/>
+      <c r="G93" s="224"/>
+      <c r="H93" s="224"/>
+      <c r="I93" s="224"/>
+      <c r="J93" s="224"/>
+      <c r="K93" s="224"/>
+      <c r="L93" s="224"/>
+      <c r="M93" s="224"/>
+      <c r="N93" s="224"/>
       <c r="O93" s="74"/>
       <c r="P93" s="75"/>
       <c r="Q93" s="96" t="s">
@@ -6841,15 +6844,15 @@
       </c>
       <c r="Y93" s="2"/>
       <c r="Z93" s="83"/>
-      <c r="AB93" s="123"/>
-      <c r="AC93" s="124"/>
-      <c r="AD93" s="124"/>
-      <c r="AE93" s="124"/>
-      <c r="AF93" s="124"/>
-      <c r="AG93" s="124"/>
-      <c r="AH93" s="134"/>
-      <c r="AI93" s="134"/>
-      <c r="AJ93" s="135"/>
+      <c r="AB93" s="238"/>
+      <c r="AC93" s="239"/>
+      <c r="AD93" s="239"/>
+      <c r="AE93" s="239"/>
+      <c r="AF93" s="239"/>
+      <c r="AG93" s="239"/>
+      <c r="AH93" s="210"/>
+      <c r="AI93" s="210"/>
+      <c r="AJ93" s="211"/>
     </row>
     <row r="94" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C94" s="73"/>
@@ -6866,17 +6869,17 @@
         <v>70</v>
       </c>
       <c r="Z94" s="83"/>
-      <c r="AB94" s="123" t="s">
+      <c r="AB94" s="238" t="s">
         <v>71</v>
       </c>
-      <c r="AC94" s="124"/>
-      <c r="AD94" s="124"/>
-      <c r="AE94" s="124"/>
-      <c r="AF94" s="124"/>
-      <c r="AG94" s="124"/>
-      <c r="AH94" s="127"/>
-      <c r="AI94" s="127"/>
-      <c r="AJ94" s="129"/>
+      <c r="AC94" s="239"/>
+      <c r="AD94" s="239"/>
+      <c r="AE94" s="239"/>
+      <c r="AF94" s="239"/>
+      <c r="AG94" s="239"/>
+      <c r="AH94" s="207"/>
+      <c r="AI94" s="207"/>
+      <c r="AJ94" s="209"/>
     </row>
     <row r="95" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B95" s="73"/>
@@ -6893,62 +6896,62 @@
       <c r="X95" s="93"/>
       <c r="Y95" s="93"/>
       <c r="Z95" s="83"/>
-      <c r="AB95" s="123"/>
-      <c r="AC95" s="124"/>
-      <c r="AD95" s="124"/>
-      <c r="AE95" s="124"/>
-      <c r="AF95" s="124"/>
-      <c r="AG95" s="124"/>
-      <c r="AH95" s="127"/>
-      <c r="AI95" s="127"/>
-      <c r="AJ95" s="129"/>
+      <c r="AB95" s="238"/>
+      <c r="AC95" s="239"/>
+      <c r="AD95" s="239"/>
+      <c r="AE95" s="239"/>
+      <c r="AF95" s="239"/>
+      <c r="AG95" s="239"/>
+      <c r="AH95" s="207"/>
+      <c r="AI95" s="207"/>
+      <c r="AJ95" s="209"/>
     </row>
     <row r="96" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="122"/>
-      <c r="C96" s="122"/>
-      <c r="D96" s="122"/>
-      <c r="E96" s="122"/>
-      <c r="F96" s="122"/>
-      <c r="G96" s="122"/>
+      <c r="B96" s="237"/>
+      <c r="C96" s="237"/>
+      <c r="D96" s="237"/>
+      <c r="E96" s="237"/>
+      <c r="F96" s="237"/>
+      <c r="G96" s="237"/>
       <c r="P96" s="75"/>
       <c r="Q96" s="96" t="s">
         <v>73</v>
       </c>
       <c r="Z96" s="83"/>
       <c r="AA96" s="105"/>
-      <c r="AB96" s="123" t="s">
+      <c r="AB96" s="238" t="s">
         <v>74</v>
       </c>
-      <c r="AC96" s="124"/>
-      <c r="AD96" s="124"/>
-      <c r="AE96" s="124"/>
-      <c r="AF96" s="124"/>
-      <c r="AG96" s="124"/>
-      <c r="AH96" s="127"/>
-      <c r="AI96" s="127"/>
-      <c r="AJ96" s="129"/>
+      <c r="AC96" s="239"/>
+      <c r="AD96" s="239"/>
+      <c r="AE96" s="239"/>
+      <c r="AF96" s="239"/>
+      <c r="AG96" s="239"/>
+      <c r="AH96" s="207"/>
+      <c r="AI96" s="207"/>
+      <c r="AJ96" s="209"/>
     </row>
     <row r="97" spans="1:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B97" s="122"/>
-      <c r="C97" s="122"/>
-      <c r="D97" s="122"/>
-      <c r="E97" s="122"/>
-      <c r="F97" s="122"/>
-      <c r="G97" s="122"/>
+      <c r="B97" s="237"/>
+      <c r="C97" s="237"/>
+      <c r="D97" s="237"/>
+      <c r="E97" s="237"/>
+      <c r="F97" s="237"/>
+      <c r="G97" s="237"/>
       <c r="P97" s="75"/>
       <c r="Q97" s="96" t="s">
         <v>75</v>
       </c>
       <c r="Z97" s="83"/>
-      <c r="AB97" s="125"/>
-      <c r="AC97" s="126"/>
-      <c r="AD97" s="126"/>
-      <c r="AE97" s="126"/>
-      <c r="AF97" s="126"/>
-      <c r="AG97" s="126"/>
-      <c r="AH97" s="128"/>
-      <c r="AI97" s="128"/>
-      <c r="AJ97" s="130"/>
+      <c r="AB97" s="240"/>
+      <c r="AC97" s="241"/>
+      <c r="AD97" s="241"/>
+      <c r="AE97" s="241"/>
+      <c r="AF97" s="241"/>
+      <c r="AG97" s="241"/>
+      <c r="AH97" s="242"/>
+      <c r="AI97" s="242"/>
+      <c r="AJ97" s="243"/>
     </row>
     <row r="98" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B98" s="2"/>
@@ -6994,23 +6997,21 @@
       <c r="B101" s="108"/>
       <c r="C101" s="108"/>
       <c r="P101" s="75"/>
-      <c r="Q101" s="131" t="s">
+      <c r="Q101" s="198" t="s">
         <v>80</v>
       </c>
-      <c r="R101" s="132"/>
-      <c r="S101" s="132"/>
-      <c r="T101" s="132"/>
-      <c r="U101" s="132"/>
-      <c r="V101" s="132"/>
-      <c r="W101" s="132"/>
-      <c r="X101" s="132"/>
-      <c r="Y101" s="132"/>
-      <c r="Z101" s="133"/>
-      <c r="AD101" s="30" t="s">
-        <v>81</v>
-      </c>
+      <c r="R101" s="199"/>
+      <c r="S101" s="199"/>
+      <c r="T101" s="199"/>
+      <c r="U101" s="199"/>
+      <c r="V101" s="199"/>
+      <c r="W101" s="199"/>
+      <c r="X101" s="199"/>
+      <c r="Y101" s="199"/>
+      <c r="Z101" s="244"/>
+      <c r="AD101" s="30"/>
       <c r="AE101" s="30"/>
-      <c r="AF101" s="30"/>
+      <c r="AF101" s="122"/>
       <c r="AG101" s="30"/>
       <c r="AH101" s="30"/>
       <c r="AI101" s="109"/>
@@ -7019,18 +7020,18 @@
       <c r="B102" s="108"/>
       <c r="C102" s="108"/>
       <c r="P102" s="75"/>
-      <c r="Q102" s="131"/>
-      <c r="R102" s="132"/>
-      <c r="S102" s="132"/>
-      <c r="T102" s="132"/>
-      <c r="U102" s="132"/>
-      <c r="V102" s="132"/>
-      <c r="W102" s="132"/>
-      <c r="X102" s="132"/>
-      <c r="Y102" s="132"/>
-      <c r="Z102" s="133"/>
+      <c r="Q102" s="198"/>
+      <c r="R102" s="199"/>
+      <c r="S102" s="199"/>
+      <c r="T102" s="199"/>
+      <c r="U102" s="199"/>
+      <c r="V102" s="199"/>
+      <c r="W102" s="199"/>
+      <c r="X102" s="199"/>
+      <c r="Y102" s="199"/>
+      <c r="Z102" s="244"/>
       <c r="AC102" s="110" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD102" s="107"/>
       <c r="AF102" s="71"/>
@@ -7041,7 +7042,7 @@
       <c r="B103" s="108"/>
       <c r="C103" s="108"/>
       <c r="Q103" s="96" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z103" s="111"/>
     </row>
@@ -7049,11 +7050,11 @@
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="Q104" s="92" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Z104" s="111"/>
       <c r="AB104" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AD104" s="104"/>
       <c r="AE104" s="107"/>
@@ -7062,30 +7063,30 @@
       <c r="AH104" s="104"/>
     </row>
     <row r="105" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="121" t="s">
-        <v>86</v>
-      </c>
-      <c r="B105" s="121"/>
+      <c r="A105" s="236" t="s">
+        <v>85</v>
+      </c>
+      <c r="B105" s="236"/>
       <c r="C105" s="108"/>
       <c r="Q105" s="96" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z105" s="111"/>
       <c r="AD105" s="30" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE105" s="30"/>
-      <c r="AF105" s="30"/>
+      <c r="AF105" s="121"/>
       <c r="AG105" s="30"/>
       <c r="AH105" s="30"/>
       <c r="AI105" s="30"/>
     </row>
     <row r="106" spans="1:36" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="121"/>
-      <c r="B106" s="121"/>
+      <c r="A106" s="236"/>
+      <c r="B106" s="236"/>
       <c r="C106" s="108"/>
       <c r="Q106" s="112" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="R106" s="70"/>
       <c r="S106" s="70"/>
@@ -7099,7 +7100,7 @@
       <c r="AD106" s="104"/>
       <c r="AE106" s="104"/>
       <c r="AF106" s="104" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AG106" s="104"/>
       <c r="AH106" s="104"/>
@@ -7108,83 +7109,51 @@
     </row>
   </sheetData>
   <mergeCells count="142">
-    <mergeCell ref="A2:AJ2"/>
-    <mergeCell ref="A3:AJ3"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="Q6:W6"/>
-    <mergeCell ref="X6:AC6"/>
-    <mergeCell ref="C8:O8"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="Z8:AB8"/>
-    <mergeCell ref="AC8:AH8"/>
-    <mergeCell ref="A10:C13"/>
-    <mergeCell ref="D10:AB10"/>
-    <mergeCell ref="AC10:AD11"/>
-    <mergeCell ref="AE10:AJ13"/>
-    <mergeCell ref="AC12:AC13"/>
-    <mergeCell ref="AE19:AJ19"/>
-    <mergeCell ref="AE20:AJ20"/>
-    <mergeCell ref="AE21:AJ21"/>
-    <mergeCell ref="AE22:AJ22"/>
-    <mergeCell ref="AE23:AJ23"/>
-    <mergeCell ref="AE24:AJ24"/>
-    <mergeCell ref="AD12:AD13"/>
-    <mergeCell ref="AE14:AJ14"/>
-    <mergeCell ref="AE15:AJ15"/>
-    <mergeCell ref="AE16:AJ16"/>
-    <mergeCell ref="AE17:AJ17"/>
-    <mergeCell ref="AE18:AJ18"/>
-    <mergeCell ref="AE31:AJ31"/>
-    <mergeCell ref="AE53:AJ53"/>
-    <mergeCell ref="AE54:AJ54"/>
-    <mergeCell ref="AE55:AJ55"/>
-    <mergeCell ref="AE32:AJ32"/>
-    <mergeCell ref="AE33:AJ33"/>
-    <mergeCell ref="AE34:AJ34"/>
-    <mergeCell ref="AE35:AJ35"/>
-    <mergeCell ref="AE52:AJ52"/>
-    <mergeCell ref="AE25:AJ25"/>
-    <mergeCell ref="AE26:AJ26"/>
-    <mergeCell ref="AE27:AJ27"/>
-    <mergeCell ref="AE28:AJ28"/>
-    <mergeCell ref="AE29:AJ29"/>
-    <mergeCell ref="AE30:AJ30"/>
-    <mergeCell ref="AE62:AJ62"/>
-    <mergeCell ref="AE63:AJ63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="AE64:AJ64"/>
-    <mergeCell ref="AE59:AJ59"/>
-    <mergeCell ref="AE60:AJ60"/>
-    <mergeCell ref="AE61:AJ61"/>
-    <mergeCell ref="AE56:AJ56"/>
-    <mergeCell ref="AE57:AJ57"/>
-    <mergeCell ref="AE58:AJ58"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="AE68:AJ68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="AE69:AJ69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="AE70:AJ70"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="AE65:AJ65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="AE66:AJ66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="AE67:AJ67"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="AE74:AJ74"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="AE75:AJ75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:H76"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="AE71:AJ71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="AE72:AJ72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="AE73:AJ73"/>
+    <mergeCell ref="A105:B106"/>
+    <mergeCell ref="B96:G97"/>
+    <mergeCell ref="AB96:AG97"/>
+    <mergeCell ref="AH96:AH97"/>
+    <mergeCell ref="AI96:AI97"/>
+    <mergeCell ref="AJ96:AJ97"/>
+    <mergeCell ref="Q101:Z102"/>
+    <mergeCell ref="AB92:AG93"/>
+    <mergeCell ref="AH92:AH93"/>
+    <mergeCell ref="AI92:AI93"/>
+    <mergeCell ref="AJ92:AJ93"/>
+    <mergeCell ref="B93:N93"/>
+    <mergeCell ref="AB94:AG95"/>
+    <mergeCell ref="AH94:AH95"/>
+    <mergeCell ref="AI94:AI95"/>
+    <mergeCell ref="AJ94:AJ95"/>
+    <mergeCell ref="AI88:AI89"/>
+    <mergeCell ref="AJ88:AJ89"/>
+    <mergeCell ref="A90:O91"/>
+    <mergeCell ref="AB90:AG91"/>
+    <mergeCell ref="AH90:AH91"/>
+    <mergeCell ref="AI90:AI91"/>
+    <mergeCell ref="AJ90:AJ91"/>
+    <mergeCell ref="D86:M86"/>
+    <mergeCell ref="A87:L87"/>
+    <mergeCell ref="AB87:AG87"/>
+    <mergeCell ref="A88:N89"/>
+    <mergeCell ref="AB88:AG89"/>
+    <mergeCell ref="AH88:AH89"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="D83:M83"/>
+    <mergeCell ref="AB83:AG84"/>
+    <mergeCell ref="AH83:AH84"/>
+    <mergeCell ref="AI83:AI84"/>
+    <mergeCell ref="AJ83:AJ84"/>
+    <mergeCell ref="D84:M84"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:C86"/>
+    <mergeCell ref="D85:M85"/>
+    <mergeCell ref="N85:O86"/>
+    <mergeCell ref="AB85:AG86"/>
+    <mergeCell ref="AH85:AH86"/>
+    <mergeCell ref="AI85:AI86"/>
+    <mergeCell ref="AJ85:AJ86"/>
     <mergeCell ref="A80:N80"/>
     <mergeCell ref="A81:A82"/>
     <mergeCell ref="B81:B82"/>
@@ -7205,51 +7174,83 @@
     <mergeCell ref="AI81:AI82"/>
     <mergeCell ref="AJ81:AJ82"/>
     <mergeCell ref="D82:M82"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="D83:M83"/>
-    <mergeCell ref="AB83:AG84"/>
-    <mergeCell ref="AH83:AH84"/>
-    <mergeCell ref="AI83:AI84"/>
-    <mergeCell ref="AJ83:AJ84"/>
-    <mergeCell ref="D84:M84"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:C86"/>
-    <mergeCell ref="D85:M85"/>
-    <mergeCell ref="N85:O86"/>
-    <mergeCell ref="AB85:AG86"/>
-    <mergeCell ref="AH85:AH86"/>
-    <mergeCell ref="AI85:AI86"/>
-    <mergeCell ref="AJ85:AJ86"/>
-    <mergeCell ref="AI88:AI89"/>
-    <mergeCell ref="AJ88:AJ89"/>
-    <mergeCell ref="A90:O91"/>
-    <mergeCell ref="AB90:AG91"/>
-    <mergeCell ref="AH90:AH91"/>
-    <mergeCell ref="AI90:AI91"/>
-    <mergeCell ref="AJ90:AJ91"/>
-    <mergeCell ref="D86:M86"/>
-    <mergeCell ref="A87:L87"/>
-    <mergeCell ref="AB87:AG87"/>
-    <mergeCell ref="A88:N89"/>
-    <mergeCell ref="AB88:AG89"/>
-    <mergeCell ref="AH88:AH89"/>
-    <mergeCell ref="A105:B106"/>
-    <mergeCell ref="B96:G97"/>
-    <mergeCell ref="AB96:AG97"/>
-    <mergeCell ref="AH96:AH97"/>
-    <mergeCell ref="AI96:AI97"/>
-    <mergeCell ref="AJ96:AJ97"/>
-    <mergeCell ref="Q101:Z102"/>
-    <mergeCell ref="AB92:AG93"/>
-    <mergeCell ref="AH92:AH93"/>
-    <mergeCell ref="AI92:AI93"/>
-    <mergeCell ref="AJ92:AJ93"/>
-    <mergeCell ref="B93:N93"/>
-    <mergeCell ref="AB94:AG95"/>
-    <mergeCell ref="AH94:AH95"/>
-    <mergeCell ref="AI94:AI95"/>
-    <mergeCell ref="AJ94:AJ95"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="AE74:AJ74"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="AE75:AJ75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:H76"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="AE71:AJ71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="AE72:AJ72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="AE73:AJ73"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="AE68:AJ68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="AE69:AJ69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="AE70:AJ70"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="AE65:AJ65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="AE66:AJ66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="AE67:AJ67"/>
+    <mergeCell ref="AE62:AJ62"/>
+    <mergeCell ref="AE63:AJ63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="AE64:AJ64"/>
+    <mergeCell ref="AE59:AJ59"/>
+    <mergeCell ref="AE60:AJ60"/>
+    <mergeCell ref="AE61:AJ61"/>
+    <mergeCell ref="AE56:AJ56"/>
+    <mergeCell ref="AE57:AJ57"/>
+    <mergeCell ref="AE58:AJ58"/>
+    <mergeCell ref="AE53:AJ53"/>
+    <mergeCell ref="AE54:AJ54"/>
+    <mergeCell ref="AE55:AJ55"/>
+    <mergeCell ref="AE32:AJ32"/>
+    <mergeCell ref="AE33:AJ33"/>
+    <mergeCell ref="AE34:AJ34"/>
+    <mergeCell ref="AE35:AJ35"/>
+    <mergeCell ref="AE52:AJ52"/>
+    <mergeCell ref="AE25:AJ25"/>
+    <mergeCell ref="AE26:AJ26"/>
+    <mergeCell ref="AE27:AJ27"/>
+    <mergeCell ref="AE28:AJ28"/>
+    <mergeCell ref="AE29:AJ29"/>
+    <mergeCell ref="AE30:AJ30"/>
+    <mergeCell ref="AE23:AJ23"/>
+    <mergeCell ref="AE24:AJ24"/>
+    <mergeCell ref="AD12:AD13"/>
+    <mergeCell ref="AE14:AJ14"/>
+    <mergeCell ref="AE15:AJ15"/>
+    <mergeCell ref="AE16:AJ16"/>
+    <mergeCell ref="AE17:AJ17"/>
+    <mergeCell ref="AE18:AJ18"/>
+    <mergeCell ref="AE31:AJ31"/>
+    <mergeCell ref="A10:C13"/>
+    <mergeCell ref="D10:AB10"/>
+    <mergeCell ref="AC10:AD11"/>
+    <mergeCell ref="AE10:AJ13"/>
+    <mergeCell ref="AC12:AC13"/>
+    <mergeCell ref="AE19:AJ19"/>
+    <mergeCell ref="AE20:AJ20"/>
+    <mergeCell ref="AE21:AJ21"/>
+    <mergeCell ref="AE22:AJ22"/>
+    <mergeCell ref="A2:AJ2"/>
+    <mergeCell ref="A3:AJ3"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="Q6:W6"/>
+    <mergeCell ref="X6:AC6"/>
+    <mergeCell ref="C8:O8"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="Z8:AB8"/>
+    <mergeCell ref="AC8:AH8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>